<commit_message>
ran haver pull and updated forecast sheet
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R631"/>
+  <dimension ref="A1:R632"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4784,13 +4784,13 @@
         <v>210662</v>
       </c>
       <c r="F98">
-        <v>13886961</v>
+        <v>13886963</v>
       </c>
       <c r="G98">
-        <v>11076397</v>
+        <v>11076399</v>
       </c>
       <c r="H98">
-        <v>904872</v>
+        <v>904873</v>
       </c>
       <c r="I98">
         <v>84.12000000000001</v>
@@ -4858,7 +4858,7 @@
         <v>79.84</v>
       </c>
       <c r="M99">
-        <v>8586181</v>
+        <v>8586182</v>
       </c>
       <c r="N99">
         <v>7675188</v>
@@ -5176,7 +5176,7 @@
         <v>82.49</v>
       </c>
       <c r="M105">
-        <v>8358621</v>
+        <v>8358622</v>
       </c>
       <c r="N105">
         <v>7677889</v>
@@ -6592,7 +6592,7 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935363</v>
+        <v>935378</v>
       </c>
       <c r="I132">
         <v>100.7</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14066910</v>
+        <v>14066925</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469363</v>
+        <v>14469377</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14604998</v>
+        <v>14605013</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690435</v>
+        <v>14690449</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14866894</v>
+        <v>14866909</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861412</v>
+        <v>14861427</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670804</v>
+        <v>14670818</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467029</v>
+        <v>14467044</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823731</v>
+        <v>823659</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14131809</v>
+        <v>14131823</v>
       </c>
       <c r="N140">
-        <v>8935567</v>
+        <v>8935495</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894105</v>
+        <v>13894120</v>
       </c>
       <c r="N141">
-        <v>8782082</v>
+        <v>8782010</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750012</v>
+        <v>13750027</v>
       </c>
       <c r="N142">
-        <v>8776350</v>
+        <v>8776278</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13621881</v>
+        <v>13621896</v>
       </c>
       <c r="N143">
-        <v>8836792</v>
+        <v>8836720</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042600</v>
+        <v>9042528</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395220</v>
+        <v>9395148</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716084</v>
+        <v>9716012</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916915</v>
+        <v>9916843</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176548</v>
+        <v>10176476</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402129</v>
+        <v>10402057</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586529</v>
+        <v>10586457</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834442</v>
+        <v>10834370</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -7870,7 +7870,7 @@
         <v>123.46</v>
       </c>
       <c r="J156">
-        <v>37.93</v>
+        <v>37.94</v>
       </c>
       <c r="K156">
         <v>15.57</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590397</v>
+        <v>590414</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,10 +9451,10 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9817199</v>
+        <v>9817610</v>
       </c>
       <c r="H186">
-        <v>1209108</v>
+        <v>1209130</v>
       </c>
       <c r="I186">
         <v>127.39</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13889898</v>
+        <v>13889919</v>
       </c>
       <c r="N186">
-        <v>8211202</v>
+        <v>8211219</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13966131</v>
+        <v>13966152</v>
       </c>
       <c r="N187">
-        <v>8231193</v>
+        <v>8231210</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9575,10 +9575,10 @@
         <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177364</v>
+        <v>14177385</v>
       </c>
       <c r="N188">
-        <v>8310979</v>
+        <v>8310996</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9604,7 +9604,7 @@
         <v>631919</v>
       </c>
       <c r="E189">
-        <v>204866</v>
+        <v>204865</v>
       </c>
       <c r="F189">
         <v>10180433</v>
@@ -9628,13 +9628,13 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260672</v>
+        <v>14260693</v>
       </c>
       <c r="N189">
-        <v>8315339</v>
+        <v>8315356</v>
       </c>
       <c r="O189">
-        <v>2521451</v>
+        <v>2521450</v>
       </c>
       <c r="P189">
         <v>3841</v>
@@ -9681,13 +9681,13 @@
         <v>126.79</v>
       </c>
       <c r="M190">
-        <v>14422999</v>
+        <v>14423020</v>
       </c>
       <c r="N190">
-        <v>8370920</v>
+        <v>8370937</v>
       </c>
       <c r="O190">
-        <v>2540059</v>
+        <v>2540058</v>
       </c>
       <c r="P190">
         <v>3855</v>
@@ -9707,7 +9707,7 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573545</v>
+        <v>573547</v>
       </c>
       <c r="E191">
         <v>207675</v>
@@ -9716,10 +9716,10 @@
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670414</v>
+        <v>8670436</v>
       </c>
       <c r="H191">
-        <v>1073055</v>
+        <v>1073058</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,13 +9734,13 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14528151</v>
+        <v>14528175</v>
       </c>
       <c r="N191">
-        <v>8368439</v>
+        <v>8368458</v>
       </c>
       <c r="O191">
-        <v>2551090</v>
+        <v>2551089</v>
       </c>
       <c r="P191">
         <v>3864</v>
@@ -9787,13 +9787,13 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532926</v>
+        <v>14532950</v>
       </c>
       <c r="N192">
-        <v>8290013</v>
+        <v>8290032</v>
       </c>
       <c r="O192">
-        <v>2547712</v>
+        <v>2547711</v>
       </c>
       <c r="P192">
         <v>3867</v>
@@ -9840,13 +9840,13 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761449</v>
+        <v>14761473</v>
       </c>
       <c r="N193">
-        <v>8365105</v>
+        <v>8365124</v>
       </c>
       <c r="O193">
-        <v>2572360</v>
+        <v>2572359</v>
       </c>
       <c r="P193">
         <v>3862</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729056</v>
+        <v>14729057</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,13 +9893,13 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14844130</v>
+        <v>14844154</v>
       </c>
       <c r="N194">
-        <v>8387992</v>
+        <v>8388011</v>
       </c>
       <c r="O194">
-        <v>2570160</v>
+        <v>2570159</v>
       </c>
       <c r="P194">
         <v>3869</v>
@@ -9946,13 +9946,13 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14889061</v>
+        <v>14889085</v>
       </c>
       <c r="N195">
-        <v>8325464</v>
+        <v>8325483</v>
       </c>
       <c r="O195">
-        <v>2571049</v>
+        <v>2571048</v>
       </c>
       <c r="P195">
         <v>3875</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097790</v>
+        <v>13097796</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,13 +9999,13 @@
         <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967742</v>
+        <v>14967767</v>
       </c>
       <c r="N196">
-        <v>8319960</v>
+        <v>8319979</v>
       </c>
       <c r="O196">
-        <v>2563123</v>
+        <v>2563122</v>
       </c>
       <c r="P196">
         <v>3873</v>
@@ -10052,13 +10052,13 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089887</v>
+        <v>15089911</v>
       </c>
       <c r="N197">
-        <v>8341424</v>
+        <v>8341443</v>
       </c>
       <c r="O197">
-        <v>2566578</v>
+        <v>2566577</v>
       </c>
       <c r="P197">
         <v>3878</v>
@@ -10105,13 +10105,13 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141503</v>
+        <v>15141506</v>
       </c>
       <c r="N198">
-        <v>8330305</v>
+        <v>8330307</v>
       </c>
       <c r="O198">
-        <v>2567379</v>
+        <v>2567378</v>
       </c>
       <c r="P198">
         <v>3884</v>
@@ -10134,10 +10134,10 @@
         <v>525103</v>
       </c>
       <c r="E199">
-        <v>214620</v>
+        <v>214621</v>
       </c>
       <c r="F199">
-        <v>10187302</v>
+        <v>10187305</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10158,10 +10158,10 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309047</v>
+        <v>15309050</v>
       </c>
       <c r="N199">
-        <v>8356553</v>
+        <v>8356555</v>
       </c>
       <c r="O199">
         <v>2587923</v>
@@ -10187,7 +10187,7 @@
         <v>735606</v>
       </c>
       <c r="E200">
-        <v>247051</v>
+        <v>247050</v>
       </c>
       <c r="F200">
         <v>11601024</v>
@@ -10211,13 +10211,13 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440657</v>
+        <v>15440660</v>
       </c>
       <c r="N200">
-        <v>8350572</v>
+        <v>8350574</v>
       </c>
       <c r="O200">
-        <v>2599976</v>
+        <v>2599975</v>
       </c>
       <c r="P200">
         <v>3886</v>
@@ -10264,10 +10264,10 @@
         <v>133.48</v>
       </c>
       <c r="M201">
-        <v>15510431</v>
+        <v>15510434</v>
       </c>
       <c r="N201">
-        <v>8368315</v>
+        <v>8368317</v>
       </c>
       <c r="O201">
         <v>2605553</v>
@@ -10317,10 +10317,10 @@
         <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673741</v>
+        <v>15673744</v>
       </c>
       <c r="N202">
-        <v>8381872</v>
+        <v>8381874</v>
       </c>
       <c r="O202">
         <v>2635466</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851479</v>
+        <v>9851475</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -10800,7 +10800,7 @@
         <v>7873641</v>
       </c>
       <c r="O211">
-        <v>2671978</v>
+        <v>2671977</v>
       </c>
       <c r="P211">
         <v>3950</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361140</v>
+        <v>1361144</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589052</v>
+        <v>11589074</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -33471,7 +33471,7 @@
         <v>182251</v>
       </c>
       <c r="F625">
-        <v>7672045</v>
+        <v>7672046</v>
       </c>
       <c r="G625">
         <v>6097705</v>
@@ -33515,25 +33515,25 @@
         <v>44592</v>
       </c>
       <c r="B626">
-        <v>1413899</v>
+        <v>1413965</v>
       </c>
       <c r="C626">
         <v>1917.5</v>
       </c>
       <c r="D626">
-        <v>528433</v>
+        <v>528859</v>
       </c>
       <c r="E626">
-        <v>177871</v>
+        <v>177858</v>
       </c>
       <c r="F626">
-        <v>9145054</v>
+        <v>9156916</v>
       </c>
       <c r="G626">
-        <v>7008256</v>
+        <v>7010215</v>
       </c>
       <c r="H626">
-        <v>2634737</v>
+        <v>2635461</v>
       </c>
       <c r="I626">
         <v>390.26</v>
@@ -33548,13 +33548,13 @@
         <v>352.7</v>
       </c>
       <c r="M626">
-        <v>41287840</v>
+        <v>41288564</v>
       </c>
       <c r="N626">
-        <v>7246641</v>
+        <v>7247067</v>
       </c>
       <c r="O626">
-        <v>4099379</v>
+        <v>4099366</v>
       </c>
       <c r="P626">
         <v>5219</v>
@@ -33571,25 +33571,25 @@
         <v>44620</v>
       </c>
       <c r="B627">
-        <v>905379</v>
+        <v>905422</v>
       </c>
       <c r="C627">
         <v>1898.8</v>
       </c>
       <c r="D627">
-        <v>391606</v>
+        <v>391934</v>
       </c>
       <c r="E627">
         <v>139258</v>
       </c>
       <c r="F627">
-        <v>7687791</v>
+        <v>7687898</v>
       </c>
       <c r="G627">
-        <v>6243367</v>
+        <v>6245143</v>
       </c>
       <c r="H627">
-        <v>2415448</v>
+        <v>2416130</v>
       </c>
       <c r="I627">
         <v>399.95</v>
@@ -33604,13 +33604,13 @@
         <v>355.84</v>
       </c>
       <c r="M627">
-        <v>38635131</v>
+        <v>38636537</v>
       </c>
       <c r="N627">
-        <v>6872121</v>
+        <v>6872875</v>
       </c>
       <c r="O627">
-        <v>3605431</v>
+        <v>3605418</v>
       </c>
       <c r="P627">
         <v>5212</v>
@@ -33627,28 +33627,28 @@
         <v>44651</v>
       </c>
       <c r="B628">
-        <v>892663</v>
+        <v>892685</v>
       </c>
       <c r="C628">
         <v>1723</v>
       </c>
       <c r="D628">
-        <v>369742</v>
+        <v>369746</v>
       </c>
       <c r="E628">
-        <v>168558</v>
+        <v>168559</v>
       </c>
       <c r="F628">
-        <v>7553475</v>
+        <v>7553247</v>
       </c>
       <c r="G628">
-        <v>6442421</v>
+        <v>6442398</v>
       </c>
       <c r="H628">
-        <v>2542352</v>
+        <v>2542341</v>
       </c>
       <c r="I628">
-        <v>407.11</v>
+        <v>407.99</v>
       </c>
       <c r="J628">
         <v>35.52</v>
@@ -33657,16 +33657,16 @@
         <v>16.53</v>
       </c>
       <c r="L628">
-        <v>359.75</v>
+        <v>359.81</v>
       </c>
       <c r="M628">
-        <v>35831022</v>
+        <v>35832416</v>
       </c>
       <c r="N628">
-        <v>6391881</v>
+        <v>6392639</v>
       </c>
       <c r="O628">
-        <v>3165221</v>
+        <v>3165209</v>
       </c>
       <c r="P628">
         <v>5213</v>
@@ -33683,25 +33683,25 @@
         <v>44681</v>
       </c>
       <c r="B629">
-        <v>877536</v>
+        <v>877570</v>
       </c>
       <c r="C629">
         <v>1430</v>
       </c>
       <c r="D629">
-        <v>304514</v>
+        <v>304518</v>
       </c>
       <c r="E629">
-        <v>125435</v>
+        <v>125434</v>
       </c>
       <c r="F629">
-        <v>6045274</v>
+        <v>6045368</v>
       </c>
       <c r="G629">
-        <v>4792493</v>
+        <v>4792485</v>
       </c>
       <c r="H629">
-        <v>1887964</v>
+        <v>1887960</v>
       </c>
       <c r="I629">
         <v>404</v>
@@ -33710,19 +33710,19 @@
         <v>33.89</v>
       </c>
       <c r="K629">
-        <v>17.41</v>
+        <v>17.4</v>
       </c>
       <c r="L629">
-        <v>363.4</v>
+        <v>363.47</v>
       </c>
       <c r="M629">
-        <v>33650347</v>
+        <v>33651738</v>
       </c>
       <c r="N629">
-        <v>5630122</v>
+        <v>5630884</v>
       </c>
       <c r="O629">
-        <v>2881924</v>
+        <v>2881911</v>
       </c>
       <c r="P629">
         <v>5218</v>
@@ -33731,7 +33731,7 @@
         <v>14091</v>
       </c>
       <c r="R629">
-        <v>319650</v>
+        <v>323392</v>
       </c>
     </row>
     <row r="630">
@@ -33739,25 +33739,25 @@
         <v>44712</v>
       </c>
       <c r="B630">
-        <v>859766</v>
+        <v>859776</v>
       </c>
       <c r="C630">
         <v>1349.6</v>
       </c>
       <c r="D630">
-        <v>312842</v>
+        <v>312845</v>
       </c>
       <c r="E630">
         <v>125662</v>
       </c>
       <c r="F630">
-        <v>5997528</v>
+        <v>5997619</v>
       </c>
       <c r="G630">
-        <v>4677140</v>
+        <v>4677136</v>
       </c>
       <c r="H630">
-        <v>1815690</v>
+        <v>1815689</v>
       </c>
       <c r="I630">
         <v>397.16</v>
@@ -33766,28 +33766,28 @@
         <v>32.6</v>
       </c>
       <c r="K630">
-        <v>17.42</v>
+        <v>17.41</v>
       </c>
       <c r="L630">
-        <v>367.86</v>
+        <v>367.93</v>
       </c>
       <c r="M630">
-        <v>31548472</v>
+        <v>31549861</v>
       </c>
       <c r="N630">
-        <v>5190810</v>
+        <v>5191575</v>
       </c>
       <c r="O630">
-        <v>2637041</v>
+        <v>2637028</v>
       </c>
       <c r="P630">
-        <v>5254</v>
+        <v>5258</v>
       </c>
       <c r="Q630">
-        <v>14104</v>
+        <v>14105</v>
       </c>
       <c r="R630">
-        <v>317251</v>
+        <v>320626</v>
       </c>
     </row>
     <row r="631">
@@ -33795,49 +33795,99 @@
         <v>44742</v>
       </c>
       <c r="B631">
-        <v>937491</v>
+        <v>937470</v>
+      </c>
+      <c r="C631">
+        <v>1297.8</v>
       </c>
       <c r="D631">
-        <v>327971</v>
+        <v>327913</v>
       </c>
       <c r="E631">
-        <v>106846</v>
+        <v>106376</v>
       </c>
       <c r="F631">
-        <v>5529454</v>
+        <v>5526924</v>
       </c>
       <c r="G631">
-        <v>4387469</v>
+        <v>4384756</v>
       </c>
       <c r="H631">
-        <v>1694212</v>
+        <v>1693004</v>
       </c>
       <c r="I631">
-        <v>394.7</v>
+        <v>394.65</v>
       </c>
       <c r="J631">
-        <v>31.59</v>
+        <v>31.58</v>
       </c>
       <c r="K631">
         <v>16.95</v>
       </c>
       <c r="L631">
-        <v>372.74</v>
+        <v>372.8</v>
       </c>
       <c r="M631">
-        <v>29255479</v>
+        <v>29255661</v>
       </c>
       <c r="N631">
-        <v>4860179</v>
+        <v>4860886</v>
       </c>
       <c r="O631">
-        <v>2409837</v>
+        <v>2409354</v>
       </c>
       <c r="P631">
-        <v>5253</v>
+        <v>5250</v>
       </c>
       <c r="Q631">
-        <v>14109</v>
+        <v>14116</v>
+      </c>
+      <c r="R631">
+        <v>318721</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="2">
+        <v>44773</v>
+      </c>
+      <c r="B632">
+        <v>1018530</v>
+      </c>
+      <c r="F632">
+        <v>6551392</v>
+      </c>
+      <c r="G632">
+        <v>4917713</v>
+      </c>
+      <c r="H632">
+        <v>1825095</v>
+      </c>
+      <c r="I632">
+        <v>380.45</v>
+      </c>
+      <c r="J632">
+        <v>30.93</v>
+      </c>
+      <c r="K632">
+        <v>16.54</v>
+      </c>
+      <c r="L632">
+        <v>377.26</v>
+      </c>
+      <c r="M632">
+        <v>27622875</v>
+      </c>
+      <c r="N632">
+        <v>4626533</v>
+      </c>
+      <c r="O632">
+        <v>2241562</v>
+      </c>
+      <c r="P632">
+        <v>5260</v>
+      </c>
+      <c r="Q632">
+        <v>14153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
q3 second revision, final commit
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R634"/>
+  <dimension ref="A1:R635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4784,10 +4784,10 @@
         <v>210662</v>
       </c>
       <c r="F98">
-        <v>13886962</v>
+        <v>13886960</v>
       </c>
       <c r="G98">
-        <v>11076398</v>
+        <v>11076396</v>
       </c>
       <c r="H98">
         <v>904872</v>
@@ -4858,7 +4858,7 @@
         <v>79.84</v>
       </c>
       <c r="M99">
-        <v>8586182</v>
+        <v>8586181</v>
       </c>
       <c r="N99">
         <v>7675188</v>
@@ -4911,7 +4911,7 @@
         <v>80.49</v>
       </c>
       <c r="M100">
-        <v>8552555</v>
+        <v>8552554</v>
       </c>
       <c r="N100">
         <v>7655474</v>
@@ -5017,7 +5017,7 @@
         <v>81.34999999999999</v>
       </c>
       <c r="M102">
-        <v>8469981</v>
+        <v>8469980</v>
       </c>
       <c r="N102">
         <v>7605385</v>
@@ -5176,7 +5176,7 @@
         <v>82.49</v>
       </c>
       <c r="M105">
-        <v>8358622</v>
+        <v>8358621</v>
       </c>
       <c r="N105">
         <v>7677889</v>
@@ -5388,7 +5388,7 @@
         <v>83.67</v>
       </c>
       <c r="M109">
-        <v>8212243</v>
+        <v>8212242</v>
       </c>
       <c r="N109">
         <v>7568310</v>
@@ -6592,7 +6592,7 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935377</v>
+        <v>935373</v>
       </c>
       <c r="I132">
         <v>100.7</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14066924</v>
+        <v>14066920</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469376</v>
+        <v>14469372</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14605011</v>
+        <v>14605008</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690448</v>
+        <v>14690445</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14866907</v>
+        <v>14866904</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861425</v>
+        <v>14861422</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670817</v>
+        <v>14670814</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467042</v>
+        <v>14467039</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823668</v>
+        <v>823674</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14131822</v>
+        <v>14131819</v>
       </c>
       <c r="N140">
-        <v>8935504</v>
+        <v>8935510</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894119</v>
+        <v>13894115</v>
       </c>
       <c r="N141">
-        <v>8782019</v>
+        <v>8782025</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750025</v>
+        <v>13750022</v>
       </c>
       <c r="N142">
-        <v>8776287</v>
+        <v>8776293</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13621894</v>
+        <v>13621891</v>
       </c>
       <c r="N143">
-        <v>8836729</v>
+        <v>8836735</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042537</v>
+        <v>9042543</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395157</v>
+        <v>9395163</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716021</v>
+        <v>9716027</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916852</v>
+        <v>9916858</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176485</v>
+        <v>10176491</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402066</v>
+        <v>10402072</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586466</v>
+        <v>10586472</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834379</v>
+        <v>10834385</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590429</v>
+        <v>590438</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,10 +9451,10 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9817905</v>
+        <v>9818082</v>
       </c>
       <c r="H186">
-        <v>1209134</v>
+        <v>1209143</v>
       </c>
       <c r="I186">
         <v>127.38</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13889924</v>
+        <v>13889933</v>
       </c>
       <c r="N186">
-        <v>8211234</v>
+        <v>8211243</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13966157</v>
+        <v>13966166</v>
       </c>
       <c r="N187">
-        <v>8231225</v>
+        <v>8231234</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9575,10 +9575,10 @@
         <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177390</v>
+        <v>14177399</v>
       </c>
       <c r="N188">
-        <v>8311011</v>
+        <v>8311020</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9628,10 +9628,10 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260698</v>
+        <v>14260707</v>
       </c>
       <c r="N189">
-        <v>8315371</v>
+        <v>8315380</v>
       </c>
       <c r="O189">
         <v>2521450</v>
@@ -9681,10 +9681,10 @@
         <v>126.79</v>
       </c>
       <c r="M190">
-        <v>14423025</v>
+        <v>14423034</v>
       </c>
       <c r="N190">
-        <v>8370952</v>
+        <v>8370961</v>
       </c>
       <c r="O190">
         <v>2540057</v>
@@ -9707,7 +9707,7 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573545</v>
+        <v>573544</v>
       </c>
       <c r="E191">
         <v>207675</v>
@@ -9716,10 +9716,10 @@
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670408</v>
+        <v>8670401</v>
       </c>
       <c r="H191">
-        <v>1073055</v>
+        <v>1073054</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,10 +9734,10 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14528177</v>
+        <v>14528185</v>
       </c>
       <c r="N191">
-        <v>8368471</v>
+        <v>8368479</v>
       </c>
       <c r="O191">
         <v>2551088</v>
@@ -9787,10 +9787,10 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532951</v>
+        <v>14532960</v>
       </c>
       <c r="N192">
-        <v>8290045</v>
+        <v>8290053</v>
       </c>
       <c r="O192">
         <v>2547710</v>
@@ -9840,10 +9840,10 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761475</v>
+        <v>14761483</v>
       </c>
       <c r="N193">
-        <v>8365137</v>
+        <v>8365145</v>
       </c>
       <c r="O193">
         <v>2572358</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729052</v>
+        <v>14729050</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,10 +9893,10 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14844156</v>
+        <v>14844164</v>
       </c>
       <c r="N194">
-        <v>8388024</v>
+        <v>8388032</v>
       </c>
       <c r="O194">
         <v>2570158</v>
@@ -9946,10 +9946,10 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14889086</v>
+        <v>14889094</v>
       </c>
       <c r="N195">
-        <v>8325496</v>
+        <v>8325504</v>
       </c>
       <c r="O195">
         <v>2571047</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097794</v>
+        <v>13097759</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,10 +9999,10 @@
         <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967768</v>
+        <v>14967776</v>
       </c>
       <c r="N196">
-        <v>8319992</v>
+        <v>8320000</v>
       </c>
       <c r="O196">
         <v>2563121</v>
@@ -10052,10 +10052,10 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089912</v>
+        <v>15089920</v>
       </c>
       <c r="N197">
-        <v>8341456</v>
+        <v>8341464</v>
       </c>
       <c r="O197">
         <v>2566576</v>
@@ -10105,10 +10105,10 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141503</v>
+        <v>15141502</v>
       </c>
       <c r="N198">
-        <v>8330305</v>
+        <v>8330304</v>
       </c>
       <c r="O198">
         <v>2567377</v>
@@ -10137,7 +10137,7 @@
         <v>214623</v>
       </c>
       <c r="F199">
-        <v>10187306</v>
+        <v>10187307</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10158,10 +10158,10 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309047</v>
+        <v>15309046</v>
       </c>
       <c r="N199">
-        <v>8356553</v>
+        <v>8356552</v>
       </c>
       <c r="O199">
         <v>2587924</v>
@@ -10211,10 +10211,10 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440657</v>
+        <v>15440656</v>
       </c>
       <c r="N200">
-        <v>8350572</v>
+        <v>8350571</v>
       </c>
       <c r="O200">
         <v>2599976</v>
@@ -10264,10 +10264,10 @@
         <v>133.48</v>
       </c>
       <c r="M201">
-        <v>15510431</v>
+        <v>15510430</v>
       </c>
       <c r="N201">
-        <v>8368315</v>
+        <v>8368314</v>
       </c>
       <c r="O201">
         <v>2605553</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071201</v>
+        <v>10071198</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10317,10 +10317,10 @@
         <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673741</v>
+        <v>15673740</v>
       </c>
       <c r="N202">
-        <v>8381872</v>
+        <v>8381871</v>
       </c>
       <c r="O202">
         <v>2635467</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851451</v>
+        <v>9851440</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361143</v>
+        <v>1361141</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589066</v>
+        <v>11589058</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -33459,28 +33459,28 @@
         <v>44561</v>
       </c>
       <c r="B625">
-        <v>1249531</v>
+        <v>1247376</v>
       </c>
       <c r="C625">
         <v>1632.8</v>
       </c>
       <c r="D625">
-        <v>414871</v>
+        <v>414843</v>
       </c>
       <c r="E625">
-        <v>182182</v>
+        <v>182033</v>
       </c>
       <c r="F625">
-        <v>7669547</v>
+        <v>7658471</v>
       </c>
       <c r="G625">
-        <v>6098061</v>
+        <v>6097968</v>
       </c>
       <c r="H625">
-        <v>2192522</v>
+        <v>2192492</v>
       </c>
       <c r="I625">
-        <v>376.43</v>
+        <v>376.45</v>
       </c>
       <c r="J625">
         <v>40.31</v>
@@ -33492,13 +33492,13 @@
         <v>349.78</v>
       </c>
       <c r="M625">
-        <v>44260461</v>
+        <v>44260432</v>
       </c>
       <c r="N625">
-        <v>7631632</v>
+        <v>7631604</v>
       </c>
       <c r="O625">
-        <v>4742095</v>
+        <v>4741946</v>
       </c>
       <c r="P625">
         <v>5237</v>
@@ -33515,28 +33515,28 @@
         <v>44592</v>
       </c>
       <c r="B626">
-        <v>1413668</v>
+        <v>1411078</v>
       </c>
       <c r="C626">
         <v>1917.5</v>
       </c>
       <c r="D626">
-        <v>529876</v>
+        <v>529855</v>
       </c>
       <c r="E626">
-        <v>177774</v>
+        <v>177702</v>
       </c>
       <c r="F626">
-        <v>9153312</v>
+        <v>9141591</v>
       </c>
       <c r="G626">
-        <v>7008471</v>
+        <v>7008417</v>
       </c>
       <c r="H626">
-        <v>2634696</v>
+        <v>2634682</v>
       </c>
       <c r="I626">
-        <v>390.24</v>
+        <v>390.26</v>
       </c>
       <c r="J626">
         <v>40.18</v>
@@ -33548,13 +33548,13 @@
         <v>352.67</v>
       </c>
       <c r="M626">
-        <v>41276789</v>
+        <v>41276745</v>
       </c>
       <c r="N626">
-        <v>7250663</v>
+        <v>7250614</v>
       </c>
       <c r="O626">
-        <v>4098103</v>
+        <v>4097882</v>
       </c>
       <c r="P626">
         <v>5219</v>
@@ -33571,28 +33571,28 @@
         <v>44620</v>
       </c>
       <c r="B627">
-        <v>905143</v>
+        <v>903307</v>
       </c>
       <c r="C627">
         <v>1898.8</v>
       </c>
       <c r="D627">
-        <v>392661</v>
+        <v>392635</v>
       </c>
       <c r="E627">
-        <v>139214</v>
+        <v>139177</v>
       </c>
       <c r="F627">
-        <v>7685163</v>
+        <v>7675337</v>
       </c>
       <c r="G627">
-        <v>6243758</v>
+        <v>6243755</v>
       </c>
       <c r="H627">
-        <v>2415534</v>
+        <v>2415529</v>
       </c>
       <c r="I627">
-        <v>399.94</v>
+        <v>399.95</v>
       </c>
       <c r="J627">
         <v>38.57</v>
@@ -33601,16 +33601,16 @@
         <v>16.82</v>
       </c>
       <c r="L627">
-        <v>355.81</v>
+        <v>355.82</v>
       </c>
       <c r="M627">
-        <v>38624166</v>
+        <v>38624118</v>
       </c>
       <c r="N627">
-        <v>6877198</v>
+        <v>6877123</v>
       </c>
       <c r="O627">
-        <v>3604111</v>
+        <v>3603853</v>
       </c>
       <c r="P627">
         <v>5212</v>
@@ -33627,28 +33627,28 @@
         <v>44651</v>
       </c>
       <c r="B628">
-        <v>892242</v>
+        <v>890106</v>
       </c>
       <c r="C628">
         <v>1723</v>
       </c>
       <c r="D628">
-        <v>370108</v>
+        <v>370087</v>
       </c>
       <c r="E628">
-        <v>168482</v>
+        <v>168457</v>
       </c>
       <c r="F628">
-        <v>7548038</v>
+        <v>7538477</v>
       </c>
       <c r="G628">
-        <v>6438790</v>
+        <v>6438750</v>
       </c>
       <c r="H628">
-        <v>2540724</v>
+        <v>2540715</v>
       </c>
       <c r="I628">
-        <v>407.97</v>
+        <v>407.98</v>
       </c>
       <c r="J628">
         <v>35.5</v>
@@ -33657,16 +33657,16 @@
         <v>16.51</v>
       </c>
       <c r="L628">
-        <v>359.77</v>
+        <v>359.78</v>
       </c>
       <c r="M628">
-        <v>35818429</v>
+        <v>35818370</v>
       </c>
       <c r="N628">
-        <v>6397324</v>
+        <v>6397228</v>
       </c>
       <c r="O628">
-        <v>3163825</v>
+        <v>3163542</v>
       </c>
       <c r="P628">
         <v>5213</v>
@@ -33683,28 +33683,28 @@
         <v>44681</v>
       </c>
       <c r="B629">
-        <v>877095</v>
+        <v>874137</v>
       </c>
       <c r="C629">
         <v>1430</v>
       </c>
       <c r="D629">
-        <v>304709</v>
+        <v>304699</v>
       </c>
       <c r="E629">
-        <v>125343</v>
+        <v>125345</v>
       </c>
       <c r="F629">
-        <v>6041681</v>
+        <v>6032730</v>
       </c>
       <c r="G629">
-        <v>4790100</v>
+        <v>4790066</v>
       </c>
       <c r="H629">
-        <v>1886936</v>
+        <v>1886923</v>
       </c>
       <c r="I629">
-        <v>403.98</v>
+        <v>403.99</v>
       </c>
       <c r="J629">
         <v>33.87</v>
@@ -33716,13 +33716,13 @@
         <v>363.43</v>
       </c>
       <c r="M629">
-        <v>33636726</v>
+        <v>33636655</v>
       </c>
       <c r="N629">
-        <v>5635760</v>
+        <v>5635654</v>
       </c>
       <c r="O629">
-        <v>2880436</v>
+        <v>2880155</v>
       </c>
       <c r="P629">
         <v>5218</v>
@@ -33772,13 +33772,13 @@
         <v>367.89</v>
       </c>
       <c r="M630">
-        <v>31534275</v>
+        <v>31534204</v>
       </c>
       <c r="N630">
-        <v>5196630</v>
+        <v>5196524</v>
       </c>
       <c r="O630">
-        <v>2635468</v>
+        <v>2635187</v>
       </c>
       <c r="P630">
         <v>5258</v>
@@ -33828,13 +33828,13 @@
         <v>372.77</v>
       </c>
       <c r="M631">
-        <v>29240217</v>
+        <v>29240146</v>
       </c>
       <c r="N631">
-        <v>4865517</v>
+        <v>4865411</v>
       </c>
       <c r="O631">
-        <v>2407841</v>
+        <v>2407560</v>
       </c>
       <c r="P631">
         <v>5238</v>
@@ -33851,31 +33851,31 @@
         <v>44773</v>
       </c>
       <c r="B632">
-        <v>1026178</v>
+        <v>1026150</v>
       </c>
       <c r="C632">
         <v>1442.9</v>
       </c>
       <c r="D632">
-        <v>367178</v>
+        <v>367190</v>
       </c>
       <c r="E632">
-        <v>113875</v>
+        <v>113474</v>
       </c>
       <c r="F632">
-        <v>6322433</v>
+        <v>6320919</v>
       </c>
       <c r="G632">
-        <v>4669006</v>
+        <v>4667208</v>
       </c>
       <c r="H632">
-        <v>1754749</v>
+        <v>1753875</v>
       </c>
       <c r="I632">
-        <v>384.03</v>
+        <v>383.98</v>
       </c>
       <c r="J632">
-        <v>30.83</v>
+        <v>30.82</v>
       </c>
       <c r="K632">
         <v>16.42</v>
@@ -33884,13 +33884,13 @@
         <v>377.44</v>
       </c>
       <c r="M632">
-        <v>27538757</v>
+        <v>27537812</v>
       </c>
       <c r="N632">
-        <v>4641868</v>
+        <v>4641774</v>
       </c>
       <c r="O632">
-        <v>2235451</v>
+        <v>2234769</v>
       </c>
       <c r="P632">
         <v>5246</v>
@@ -33899,7 +33899,7 @@
         <v>14157</v>
       </c>
       <c r="R632">
-        <v>331601</v>
+        <v>336811</v>
       </c>
     </row>
     <row r="633">
@@ -33907,31 +33907,31 @@
         <v>44804</v>
       </c>
       <c r="B633">
-        <v>885265</v>
+        <v>885169</v>
       </c>
       <c r="C633">
         <v>1399.5</v>
       </c>
       <c r="D633">
-        <v>355160</v>
+        <v>355131</v>
       </c>
       <c r="E633">
-        <v>120804</v>
+        <v>120402</v>
       </c>
       <c r="F633">
-        <v>6364213</v>
+        <v>6362974</v>
       </c>
       <c r="G633">
-        <v>5290199</v>
+        <v>5288548</v>
       </c>
       <c r="H633">
-        <v>2005846</v>
+        <v>2005155</v>
       </c>
       <c r="I633">
-        <v>389.97</v>
+        <v>389.96</v>
       </c>
       <c r="J633">
-        <v>30.28</v>
+        <v>30.26</v>
       </c>
       <c r="K633">
         <v>15.63</v>
@@ -33940,22 +33940,22 @@
         <v>382.63</v>
       </c>
       <c r="M633">
-        <v>26098703</v>
+        <v>26097068</v>
       </c>
       <c r="N633">
-        <v>4536583</v>
+        <v>4536460</v>
       </c>
       <c r="O633">
-        <v>2082153</v>
+        <v>2081069</v>
       </c>
       <c r="P633">
-        <v>5247</v>
+        <v>5261</v>
       </c>
       <c r="Q633">
-        <v>14198</v>
+        <v>14201</v>
       </c>
       <c r="R633">
-        <v>330337</v>
+        <v>342774</v>
       </c>
     </row>
     <row r="634">
@@ -33963,28 +33963,31 @@
         <v>44834</v>
       </c>
       <c r="B634">
-        <v>717451</v>
+        <v>718568</v>
+      </c>
+      <c r="C634">
+        <v>1218.6</v>
       </c>
       <c r="D634">
-        <v>285950</v>
+        <v>286050</v>
       </c>
       <c r="E634">
-        <v>106802</v>
+        <v>106776</v>
       </c>
       <c r="F634">
-        <v>5706132</v>
+        <v>5707588</v>
       </c>
       <c r="G634">
-        <v>4186917</v>
+        <v>4188330</v>
       </c>
       <c r="H634">
-        <v>1652775</v>
+        <v>1653091</v>
       </c>
       <c r="I634">
-        <v>403.8</v>
+        <v>403.73</v>
       </c>
       <c r="J634">
-        <v>29.44</v>
+        <v>29.42</v>
       </c>
       <c r="K634">
         <v>15.42</v>
@@ -33993,19 +33996,39 @@
         <v>387.52</v>
       </c>
       <c r="M634">
-        <v>25067483</v>
+        <v>25066164</v>
       </c>
       <c r="N634">
-        <v>4344346</v>
+        <v>4344323</v>
       </c>
       <c r="O634">
-        <v>1883339</v>
+        <v>1882229</v>
       </c>
       <c r="P634">
-        <v>5231</v>
+        <v>5261</v>
       </c>
       <c r="Q634">
-        <v>14187</v>
+        <v>14194</v>
+      </c>
+      <c r="R634">
+        <v>348166</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C635">
+        <v>1222.3</v>
+      </c>
+      <c r="P635">
+        <v>5254</v>
+      </c>
+      <c r="Q635">
+        <v>14223</v>
+      </c>
+      <c r="R635">
+        <v>348475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
q3 2nd revision, prelim data pull and haver back up
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R635"/>
+  <dimension ref="A1:R636"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -33739,28 +33739,28 @@
         <v>44712</v>
       </c>
       <c r="B630">
-        <v>859355</v>
+        <v>858243</v>
       </c>
       <c r="C630">
         <v>1349.6</v>
       </c>
       <c r="D630">
-        <v>313024</v>
+        <v>313021</v>
       </c>
       <c r="E630">
-        <v>125577</v>
+        <v>125552</v>
       </c>
       <c r="F630">
-        <v>5994282</v>
+        <v>5982003</v>
       </c>
       <c r="G630">
-        <v>4675798</v>
+        <v>4675812</v>
       </c>
       <c r="H630">
-        <v>1815114</v>
+        <v>1815116</v>
       </c>
       <c r="I630">
-        <v>397.15</v>
+        <v>397.16</v>
       </c>
       <c r="J630">
         <v>32.57</v>
@@ -33772,13 +33772,13 @@
         <v>367.89</v>
       </c>
       <c r="M630">
-        <v>31534204</v>
+        <v>31534206</v>
       </c>
       <c r="N630">
-        <v>5196524</v>
+        <v>5196521</v>
       </c>
       <c r="O630">
-        <v>2635187</v>
+        <v>2635162</v>
       </c>
       <c r="P630">
         <v>5258</v>
@@ -33795,28 +33795,28 @@
         <v>44742</v>
       </c>
       <c r="B631">
-        <v>937326</v>
+        <v>936213</v>
       </c>
       <c r="C631">
         <v>1297.8</v>
       </c>
       <c r="D631">
-        <v>327883</v>
+        <v>327875</v>
       </c>
       <c r="E631">
-        <v>106319</v>
+        <v>106283</v>
       </c>
       <c r="F631">
-        <v>5524780</v>
+        <v>5513046</v>
       </c>
       <c r="G631">
-        <v>4383369</v>
+        <v>4383367</v>
       </c>
       <c r="H631">
-        <v>1692387</v>
+        <v>1692379</v>
       </c>
       <c r="I631">
-        <v>394.63</v>
+        <v>394.65</v>
       </c>
       <c r="J631">
         <v>31.55</v>
@@ -33828,13 +33828,13 @@
         <v>372.77</v>
       </c>
       <c r="M631">
-        <v>29240146</v>
+        <v>29240140</v>
       </c>
       <c r="N631">
-        <v>4865411</v>
+        <v>4865400</v>
       </c>
       <c r="O631">
-        <v>2407560</v>
+        <v>2407499</v>
       </c>
       <c r="P631">
         <v>5238</v>
@@ -33863,7 +33863,7 @@
         <v>113474</v>
       </c>
       <c r="F632">
-        <v>6320919</v>
+        <v>6320944</v>
       </c>
       <c r="G632">
         <v>4667208</v>
@@ -33884,13 +33884,13 @@
         <v>377.44</v>
       </c>
       <c r="M632">
-        <v>27537812</v>
+        <v>27537806</v>
       </c>
       <c r="N632">
-        <v>4641774</v>
+        <v>4641763</v>
       </c>
       <c r="O632">
-        <v>2234769</v>
+        <v>2234708</v>
       </c>
       <c r="P632">
         <v>5246</v>
@@ -33907,46 +33907,46 @@
         <v>44804</v>
       </c>
       <c r="B633">
-        <v>885169</v>
+        <v>888742</v>
       </c>
       <c r="C633">
         <v>1399.5</v>
       </c>
       <c r="D633">
-        <v>355131</v>
+        <v>356591</v>
       </c>
       <c r="E633">
-        <v>120402</v>
+        <v>118733</v>
       </c>
       <c r="F633">
-        <v>6362974</v>
+        <v>6337806</v>
       </c>
       <c r="G633">
-        <v>5288548</v>
+        <v>5273207</v>
       </c>
       <c r="H633">
-        <v>2005155</v>
+        <v>2003703</v>
       </c>
       <c r="I633">
-        <v>389.96</v>
+        <v>390.7</v>
       </c>
       <c r="J633">
-        <v>30.26</v>
+        <v>30.24</v>
       </c>
       <c r="K633">
-        <v>15.63</v>
+        <v>15.62</v>
       </c>
       <c r="L633">
-        <v>382.63</v>
+        <v>382.69</v>
       </c>
       <c r="M633">
-        <v>26097068</v>
+        <v>26095610</v>
       </c>
       <c r="N633">
-        <v>4536460</v>
+        <v>4537909</v>
       </c>
       <c r="O633">
-        <v>2081069</v>
+        <v>2079339</v>
       </c>
       <c r="P633">
         <v>5261</v>
@@ -33963,72 +33963,122 @@
         <v>44834</v>
       </c>
       <c r="B634">
-        <v>718568</v>
+        <v>879662.6666666666</v>
       </c>
       <c r="C634">
-        <v>1218.6</v>
+        <v>1353.666666666667</v>
       </c>
       <c r="D634">
-        <v>286050</v>
+        <v>336686</v>
       </c>
       <c r="E634">
-        <v>106776</v>
+        <v>111378</v>
       </c>
       <c r="F634">
-        <v>5707588</v>
+        <v>6115849.666666667</v>
       </c>
       <c r="G634">
-        <v>4188330</v>
+        <v>4705372</v>
       </c>
       <c r="H634">
-        <v>1653091</v>
+        <v>1803645</v>
       </c>
       <c r="I634">
-        <v>403.73</v>
+        <v>393.14</v>
       </c>
       <c r="J634">
-        <v>29.42</v>
+        <v>30.12666666666667</v>
       </c>
       <c r="K634">
-        <v>15.42</v>
+        <v>15.81666666666667</v>
       </c>
       <c r="L634">
-        <v>387.52</v>
+        <v>382.59</v>
       </c>
       <c r="M634">
-        <v>25066164</v>
+        <v>26232795.66666667</v>
       </c>
       <c r="N634">
-        <v>4344323</v>
+        <v>4508557</v>
       </c>
       <c r="O634">
-        <v>1882229</v>
+        <v>2063232.333333333</v>
       </c>
       <c r="P634">
-        <v>5261</v>
+        <v>5260</v>
       </c>
       <c r="Q634">
-        <v>14194</v>
+        <v>14186</v>
       </c>
       <c r="R634">
-        <v>348166</v>
+        <v>342583.6666666667</v>
       </c>
     </row>
     <row r="635">
       <c r="A635" s="2">
         <v>44865</v>
       </c>
+      <c r="B635">
+        <v>826695</v>
+      </c>
       <c r="C635">
         <v>1222.3</v>
       </c>
+      <c r="D635">
+        <v>294264</v>
+      </c>
+      <c r="E635">
+        <v>114228</v>
+      </c>
+      <c r="F635">
+        <v>5627721</v>
+      </c>
+      <c r="G635">
+        <v>4359116</v>
+      </c>
+      <c r="H635">
+        <v>1732508</v>
+      </c>
+      <c r="I635">
+        <v>407.33</v>
+      </c>
+      <c r="J635">
+        <v>29.88</v>
+      </c>
+      <c r="K635">
+        <v>15.06</v>
+      </c>
+      <c r="L635">
+        <v>392.77</v>
+      </c>
+      <c r="M635">
+        <v>24541990</v>
+      </c>
+      <c r="N635">
+        <v>4286306</v>
+      </c>
+      <c r="O635">
+        <v>1683902</v>
+      </c>
       <c r="P635">
-        <v>5254</v>
+        <v>5273</v>
       </c>
       <c r="Q635">
-        <v>14223</v>
+        <v>14231</v>
       </c>
       <c r="R635">
         <v>348475</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="2">
+        <v>44895</v>
+      </c>
+      <c r="P636">
+        <v>5284</v>
+      </c>
+      <c r="Q636">
+        <v>14263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new haver pull backup -- pulled Q4
commented out sections of haver pull backup, updated haver backup sheet, prelim pull of 2022 Q4 data
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -34130,11 +34130,56 @@
       <c r="A637" s="2">
         <v>44926</v>
       </c>
+      <c r="B637">
+        <v>998172.3333333334</v>
+      </c>
+      <c r="C637">
+        <v>1375.4</v>
+      </c>
+      <c r="D637">
+        <v>370949.6666666667</v>
+      </c>
+      <c r="E637">
+        <v>113731.3333333333</v>
+      </c>
+      <c r="F637">
+        <v>5970677.333333333</v>
+      </c>
+      <c r="G637">
+        <v>4782585.333333333</v>
+      </c>
+      <c r="H637">
+        <v>1947630.333333333</v>
+      </c>
+      <c r="I637">
+        <v>415.3933333333333</v>
+      </c>
+      <c r="J637">
+        <v>30.54333333333333</v>
+      </c>
+      <c r="K637">
+        <v>14.60333333333333</v>
+      </c>
+      <c r="L637">
+        <v>397.1166666666667</v>
+      </c>
+      <c r="M637">
+        <v>24341787.66666667</v>
+      </c>
+      <c r="N637">
+        <v>4322390</v>
+      </c>
+      <c r="O637">
+        <v>1596513</v>
+      </c>
       <c r="P637">
-        <v>5269</v>
+        <v>5277</v>
       </c>
       <c r="Q637">
-        <v>14297</v>
+        <v>14270.33333333333</v>
+      </c>
+      <c r="R637">
+        <v>352213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to forecast sheet in preparation for our Friday FIM release!
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R639"/>
+  <dimension ref="A1:R640"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2832,7 +2832,7 @@
         <v>745011</v>
       </c>
       <c r="I61">
-        <v>67.24</v>
+        <v>67.23999999999999</v>
       </c>
       <c r="J61">
         <v>30.96</v>
@@ -3265,7 +3265,7 @@
         <v>14.29</v>
       </c>
       <c r="L69">
-        <v>68.74</v>
+        <v>68.73999999999999</v>
       </c>
       <c r="M69">
         <v>10944048</v>
@@ -3362,7 +3362,7 @@
         <v>757012</v>
       </c>
       <c r="I71">
-        <v>72.37000000000001</v>
+        <v>72.37</v>
       </c>
       <c r="J71">
         <v>37.4</v>
@@ -4687,7 +4687,7 @@
         <v>597933</v>
       </c>
       <c r="I96">
-        <v>80.24</v>
+        <v>80.23999999999999</v>
       </c>
       <c r="J96">
         <v>32.98</v>
@@ -4793,7 +4793,7 @@
         <v>904872</v>
       </c>
       <c r="I98">
-        <v>84.12000000000001</v>
+        <v>84.12</v>
       </c>
       <c r="J98">
         <v>32.33</v>
@@ -4908,7 +4908,7 @@
         <v>14.26</v>
       </c>
       <c r="L100">
-        <v>80.49</v>
+        <v>80.48999999999999</v>
       </c>
       <c r="M100">
         <v>8552554</v>
@@ -5067,7 +5067,7 @@
         <v>13.87</v>
       </c>
       <c r="L103">
-        <v>81.74</v>
+        <v>81.73999999999999</v>
       </c>
       <c r="M103">
         <v>8390319</v>
@@ -5120,7 +5120,7 @@
         <v>13.74</v>
       </c>
       <c r="L104">
-        <v>82.12000000000001</v>
+        <v>82.12</v>
       </c>
       <c r="M104">
         <v>8353744</v>
@@ -5173,7 +5173,7 @@
         <v>13.57</v>
       </c>
       <c r="L105">
-        <v>82.49</v>
+        <v>82.48999999999999</v>
       </c>
       <c r="M105">
         <v>8358621</v>
@@ -5544,7 +5544,7 @@
         <v>13.21</v>
       </c>
       <c r="L112">
-        <v>85.12000000000001</v>
+        <v>85.12</v>
       </c>
       <c r="M112">
         <v>8256015</v>
@@ -5641,7 +5641,7 @@
         <v>725229</v>
       </c>
       <c r="I114">
-        <v>88.37000000000001</v>
+        <v>88.37</v>
       </c>
       <c r="J114">
         <v>25.87</v>
@@ -5968,7 +5968,7 @@
         <v>13.08</v>
       </c>
       <c r="L120">
-        <v>88.99</v>
+        <v>88.98999999999999</v>
       </c>
       <c r="M120">
         <v>9066829</v>
@@ -6277,7 +6277,7 @@
         <v>1196836</v>
       </c>
       <c r="I126">
-        <v>99.74</v>
+        <v>99.73999999999999</v>
       </c>
       <c r="J126">
         <v>28.31</v>
@@ -6592,10 +6592,10 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935557</v>
+        <v>935495</v>
       </c>
       <c r="I132">
-        <v>100.72</v>
+        <v>100.71</v>
       </c>
       <c r="J132">
         <v>32.75</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14067104</v>
+        <v>14067042</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469556</v>
+        <v>14469495</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14605192</v>
+        <v>14605130</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690628</v>
+        <v>14690567</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14867088</v>
+        <v>14867026</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861606</v>
+        <v>14861544</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670998</v>
+        <v>14670936</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467223</v>
+        <v>14467161</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823701</v>
+        <v>823711</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14132003</v>
+        <v>14131941</v>
       </c>
       <c r="N140">
-        <v>8935537</v>
+        <v>8935547</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894299</v>
+        <v>13894237</v>
       </c>
       <c r="N141">
-        <v>8782052</v>
+        <v>8782062</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750206</v>
+        <v>13750144</v>
       </c>
       <c r="N142">
-        <v>8776320</v>
+        <v>8776330</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13622075</v>
+        <v>13622013</v>
       </c>
       <c r="N143">
-        <v>8836762</v>
+        <v>8836772</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042570</v>
+        <v>9042580</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395190</v>
+        <v>9395200</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716054</v>
+        <v>9716064</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916885</v>
+        <v>9916895</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176518</v>
+        <v>10176528</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402099</v>
+        <v>10402109</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586499</v>
+        <v>10586509</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834412</v>
+        <v>10834422</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590478</v>
+        <v>590485</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,10 +9451,10 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9818625</v>
+        <v>9818740</v>
       </c>
       <c r="H186">
-        <v>1208992</v>
+        <v>1208967</v>
       </c>
       <c r="I186">
         <v>127.36</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13889781</v>
+        <v>13889756</v>
       </c>
       <c r="N186">
-        <v>8211283</v>
+        <v>8211290</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13966014</v>
+        <v>13965989</v>
       </c>
       <c r="N187">
-        <v>8231274</v>
+        <v>8231281</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9575,10 +9575,10 @@
         <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177248</v>
+        <v>14177222</v>
       </c>
       <c r="N188">
-        <v>8311060</v>
+        <v>8311067</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9628,10 +9628,10 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260555</v>
+        <v>14260530</v>
       </c>
       <c r="N189">
-        <v>8315420</v>
+        <v>8315427</v>
       </c>
       <c r="O189">
         <v>2521451</v>
@@ -9678,13 +9678,13 @@
         <v>14.06</v>
       </c>
       <c r="L190">
-        <v>126.79</v>
+        <v>126.78</v>
       </c>
       <c r="M190">
-        <v>14422882</v>
+        <v>14422857</v>
       </c>
       <c r="N190">
-        <v>8371001</v>
+        <v>8371008</v>
       </c>
       <c r="O190">
         <v>2540057</v>
@@ -9707,19 +9707,19 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573547</v>
+        <v>573551</v>
       </c>
       <c r="E191">
-        <v>207670</v>
+        <v>207672</v>
       </c>
       <c r="F191">
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670448</v>
+        <v>8670501</v>
       </c>
       <c r="H191">
-        <v>1073070</v>
+        <v>1073073</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,13 +9734,13 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14528050</v>
+        <v>14528027</v>
       </c>
       <c r="N191">
-        <v>8368522</v>
+        <v>8368533</v>
       </c>
       <c r="O191">
-        <v>2551083</v>
+        <v>2551085</v>
       </c>
       <c r="P191">
         <v>3864</v>
@@ -9787,13 +9787,13 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532825</v>
+        <v>14532802</v>
       </c>
       <c r="N192">
-        <v>8290096</v>
+        <v>8290107</v>
       </c>
       <c r="O192">
-        <v>2547705</v>
+        <v>2547707</v>
       </c>
       <c r="P192">
         <v>3867</v>
@@ -9840,13 +9840,13 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761348</v>
+        <v>14761325</v>
       </c>
       <c r="N193">
-        <v>8365188</v>
+        <v>8365199</v>
       </c>
       <c r="O193">
-        <v>2572353</v>
+        <v>2572355</v>
       </c>
       <c r="P193">
         <v>3862</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729036</v>
+        <v>14729039</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,13 +9893,13 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14844029</v>
+        <v>14844006</v>
       </c>
       <c r="N194">
-        <v>8388075</v>
+        <v>8388086</v>
       </c>
       <c r="O194">
-        <v>2570153</v>
+        <v>2570155</v>
       </c>
       <c r="P194">
         <v>3869</v>
@@ -9946,13 +9946,13 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14888959</v>
+        <v>14888937</v>
       </c>
       <c r="N195">
-        <v>8325547</v>
+        <v>8325558</v>
       </c>
       <c r="O195">
-        <v>2571042</v>
+        <v>2571044</v>
       </c>
       <c r="P195">
         <v>3875</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097784</v>
+        <v>13097731</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,13 +9999,13 @@
         <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967641</v>
+        <v>14967619</v>
       </c>
       <c r="N196">
-        <v>8320043</v>
+        <v>8320054</v>
       </c>
       <c r="O196">
-        <v>2563116</v>
+        <v>2563118</v>
       </c>
       <c r="P196">
         <v>3873</v>
@@ -10052,13 +10052,13 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089786</v>
+        <v>15089763</v>
       </c>
       <c r="N197">
-        <v>8341507</v>
+        <v>8341518</v>
       </c>
       <c r="O197">
-        <v>2566571</v>
+        <v>2566573</v>
       </c>
       <c r="P197">
         <v>3878</v>
@@ -10105,13 +10105,13 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141519</v>
+        <v>15141521</v>
       </c>
       <c r="N198">
-        <v>8330307</v>
+        <v>8330311</v>
       </c>
       <c r="O198">
-        <v>2567372</v>
+        <v>2567374</v>
       </c>
       <c r="P198">
         <v>3884</v>
@@ -10137,7 +10137,7 @@
         <v>214628</v>
       </c>
       <c r="F199">
-        <v>10187312</v>
+        <v>10187313</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10158,13 +10158,13 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309063</v>
+        <v>15309065</v>
       </c>
       <c r="N199">
-        <v>8356555</v>
+        <v>8356559</v>
       </c>
       <c r="O199">
-        <v>2587924</v>
+        <v>2587926</v>
       </c>
       <c r="P199">
         <v>3887</v>
@@ -10211,13 +10211,13 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440672</v>
+        <v>15440675</v>
       </c>
       <c r="N200">
-        <v>8350574</v>
+        <v>8350578</v>
       </c>
       <c r="O200">
-        <v>2599976</v>
+        <v>2599978</v>
       </c>
       <c r="P200">
         <v>3886</v>
@@ -10264,13 +10264,13 @@
         <v>133.49</v>
       </c>
       <c r="M201">
-        <v>15510447</v>
+        <v>15510449</v>
       </c>
       <c r="N201">
-        <v>8368317</v>
+        <v>8368321</v>
       </c>
       <c r="O201">
-        <v>2605551</v>
+        <v>2605553</v>
       </c>
       <c r="P201">
         <v>3887</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071173</v>
+        <v>10071177</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10317,13 +10317,13 @@
         <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673757</v>
+        <v>15673759</v>
       </c>
       <c r="N202">
-        <v>8381874</v>
+        <v>8381878</v>
       </c>
       <c r="O202">
-        <v>2635466</v>
+        <v>2635468</v>
       </c>
       <c r="P202">
         <v>3895</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851387</v>
+        <v>9851394</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361152</v>
+        <v>1361128</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589053</v>
+        <v>11588963</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -33530,13 +33530,13 @@
         <v>9141591</v>
       </c>
       <c r="G626">
-        <v>7008417</v>
+        <v>7009776</v>
       </c>
       <c r="H626">
-        <v>2634682</v>
+        <v>2635174</v>
       </c>
       <c r="I626">
-        <v>390.26</v>
+        <v>390.25</v>
       </c>
       <c r="J626">
         <v>40.18</v>
@@ -33548,7 +33548,7 @@
         <v>352.67</v>
       </c>
       <c r="M626">
-        <v>41276269</v>
+        <v>41276761</v>
       </c>
       <c r="N626">
         <v>7250472</v>
@@ -33604,7 +33604,7 @@
         <v>355.82</v>
       </c>
       <c r="M627">
-        <v>38623642</v>
+        <v>38624133</v>
       </c>
       <c r="N627">
         <v>6876981</v>
@@ -33660,7 +33660,7 @@
         <v>359.78</v>
       </c>
       <c r="M628">
-        <v>35817894</v>
+        <v>35818386</v>
       </c>
       <c r="N628">
         <v>6397086</v>
@@ -33716,7 +33716,7 @@
         <v>363.43</v>
       </c>
       <c r="M629">
-        <v>33636179</v>
+        <v>33636671</v>
       </c>
       <c r="N629">
         <v>5635512</v>
@@ -33772,7 +33772,7 @@
         <v>367.89</v>
       </c>
       <c r="M630">
-        <v>31533730</v>
+        <v>31534221</v>
       </c>
       <c r="N630">
         <v>5196379</v>
@@ -33828,7 +33828,7 @@
         <v>372.77</v>
       </c>
       <c r="M631">
-        <v>29239664</v>
+        <v>29240156</v>
       </c>
       <c r="N631">
         <v>4865258</v>
@@ -33884,7 +33884,7 @@
         <v>377.44</v>
       </c>
       <c r="M632">
-        <v>27537330</v>
+        <v>27537822</v>
       </c>
       <c r="N632">
         <v>4641621</v>
@@ -33940,7 +33940,7 @@
         <v>382.69</v>
       </c>
       <c r="M633">
-        <v>26108134</v>
+        <v>26108626</v>
       </c>
       <c r="N633">
         <v>4537767</v>
@@ -33996,7 +33996,7 @@
         <v>387.61</v>
       </c>
       <c r="M634">
-        <v>25081944</v>
+        <v>25082436</v>
       </c>
       <c r="N634">
         <v>4347817</v>
@@ -34052,7 +34052,7 @@
         <v>392.67</v>
       </c>
       <c r="M635">
-        <v>24558962</v>
+        <v>24559454</v>
       </c>
       <c r="N635">
         <v>4290001</v>
@@ -34087,7 +34087,7 @@
         <v>112215</v>
       </c>
       <c r="F636">
-        <v>5707447</v>
+        <v>5707460</v>
       </c>
       <c r="G636">
         <v>4583847</v>
@@ -34108,7 +34108,7 @@
         <v>397.24</v>
       </c>
       <c r="M636">
-        <v>24210257</v>
+        <v>24210749</v>
       </c>
       <c r="N636">
         <v>4314272</v>
@@ -34143,7 +34143,7 @@
         <v>114751</v>
       </c>
       <c r="F637">
-        <v>6576864</v>
+        <v>6576878</v>
       </c>
       <c r="G637">
         <v>5404792</v>
@@ -34164,7 +34164,7 @@
         <v>401.44</v>
       </c>
       <c r="M637">
-        <v>24256144</v>
+        <v>24256635</v>
       </c>
       <c r="N637">
         <v>4362897</v>
@@ -34179,7 +34179,7 @@
         <v>14370</v>
       </c>
       <c r="R637">
-        <v>356463</v>
+        <v>359372</v>
       </c>
     </row>
     <row r="638">
@@ -34196,7 +34196,7 @@
         <v>650635</v>
       </c>
       <c r="E638">
-        <v>139672</v>
+        <v>140555</v>
       </c>
       <c r="F638">
         <v>8985963</v>
@@ -34211,7 +34211,7 @@
         <v>430.2</v>
       </c>
       <c r="J638">
-        <v>31.9</v>
+        <v>31.92</v>
       </c>
       <c r="K638">
         <v>13.91</v>
@@ -34226,16 +34226,16 @@
         <v>4483677</v>
       </c>
       <c r="O638">
-        <v>1480802</v>
+        <v>1481685</v>
       </c>
       <c r="P638">
-        <v>5162</v>
+        <v>5156</v>
       </c>
       <c r="Q638">
-        <v>14406</v>
+        <v>14408</v>
       </c>
       <c r="R638">
-        <v>351554</v>
+        <v>360187</v>
       </c>
     </row>
     <row r="639">
@@ -34245,11 +34245,14 @@
       <c r="B639">
         <v>893566</v>
       </c>
+      <c r="C639">
+        <v>1870.1</v>
+      </c>
       <c r="D639">
         <v>467142</v>
       </c>
       <c r="E639">
-        <v>118210</v>
+        <v>118685</v>
       </c>
       <c r="F639">
         <v>7771440</v>
@@ -34264,7 +34267,7 @@
         <v>437.68</v>
       </c>
       <c r="J639">
-        <v>32.17</v>
+        <v>32.2</v>
       </c>
       <c r="K639">
         <v>13.75</v>
@@ -34279,13 +34282,69 @@
         <v>4558184</v>
       </c>
       <c r="O639">
-        <v>1459835</v>
+        <v>1461193</v>
       </c>
       <c r="P639">
-        <v>5164</v>
+        <v>5171</v>
       </c>
       <c r="Q639">
-        <v>14443</v>
+        <v>14444</v>
+      </c>
+      <c r="R639">
+        <v>359010</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="2">
+        <v>45016</v>
+      </c>
+      <c r="B640">
+        <v>986619</v>
+      </c>
+      <c r="C640">
+        <v>1852.7</v>
+      </c>
+      <c r="D640">
+        <v>410200</v>
+      </c>
+      <c r="E640">
+        <v>130478</v>
+      </c>
+      <c r="F640">
+        <v>7973206</v>
+      </c>
+      <c r="G640">
+        <v>6870522</v>
+      </c>
+      <c r="H640">
+        <v>2978415</v>
+      </c>
+      <c r="I640">
+        <v>441.25</v>
+      </c>
+      <c r="J640">
+        <v>32.73</v>
+      </c>
+      <c r="K640">
+        <v>13.72</v>
+      </c>
+      <c r="L640">
+        <v>413.68</v>
+      </c>
+      <c r="M640">
+        <v>25582401</v>
+      </c>
+      <c r="N640">
+        <v>4598297</v>
+      </c>
+      <c r="O640">
+        <v>1423214</v>
+      </c>
+      <c r="P640">
+        <v>5184</v>
+      </c>
+      <c r="Q640">
+        <v>14470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Haver pull August 2023
Haverpull was pulled. Only thing that looks down is state non-corporate, which is all Haver codes.
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R643"/>
+  <dimension ref="A1:R644"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6592,7 +6592,7 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935438</v>
+        <v>935387</v>
       </c>
       <c r="I132">
         <v>100.7</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14066985</v>
+        <v>14066934</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469438</v>
+        <v>14469387</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14605073</v>
+        <v>14605022</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690510</v>
+        <v>14690459</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14866969</v>
+        <v>14866918</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861487</v>
+        <v>14861436</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670879</v>
+        <v>14670828</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467104</v>
+        <v>14467053</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823741</v>
+        <v>823667</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14131884</v>
+        <v>14131833</v>
       </c>
       <c r="N140">
-        <v>8935577</v>
+        <v>8935503</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894180</v>
+        <v>13894129</v>
       </c>
       <c r="N141">
-        <v>8782092</v>
+        <v>8782018</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750087</v>
+        <v>13750036</v>
       </c>
       <c r="N142">
-        <v>8776360</v>
+        <v>8776286</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13621956</v>
+        <v>13621905</v>
       </c>
       <c r="N143">
-        <v>8836802</v>
+        <v>8836728</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042610</v>
+        <v>9042536</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395230</v>
+        <v>9395156</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716094</v>
+        <v>9716020</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916925</v>
+        <v>9916851</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176558</v>
+        <v>10176484</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402139</v>
+        <v>10402065</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586539</v>
+        <v>10586465</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834452</v>
+        <v>10834378</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -7870,7 +7870,7 @@
         <v>123.46</v>
       </c>
       <c r="J156">
-        <v>37.93</v>
+        <v>37.94</v>
       </c>
       <c r="K156">
         <v>15.57</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590389</v>
+        <v>590412</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,13 +9451,13 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9817128</v>
+        <v>9817665</v>
       </c>
       <c r="H186">
-        <v>1209245</v>
+        <v>1209170</v>
       </c>
       <c r="I186">
-        <v>127.41</v>
+        <v>127.39</v>
       </c>
       <c r="J186">
         <v>32.49</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13890034</v>
+        <v>13889959</v>
       </c>
       <c r="N186">
-        <v>8211194</v>
+        <v>8211217</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13966267</v>
+        <v>13966192</v>
       </c>
       <c r="N187">
-        <v>8231185</v>
+        <v>8231208</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9572,13 +9572,13 @@
         <v>14.01</v>
       </c>
       <c r="L188">
-        <v>125.9</v>
+        <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177500</v>
+        <v>14177425</v>
       </c>
       <c r="N188">
-        <v>8310971</v>
+        <v>8310994</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9628,10 +9628,10 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260808</v>
+        <v>14260733</v>
       </c>
       <c r="N189">
-        <v>8315331</v>
+        <v>8315354</v>
       </c>
       <c r="O189">
         <v>2521450</v>
@@ -9681,10 +9681,10 @@
         <v>126.79</v>
       </c>
       <c r="M190">
-        <v>14423135</v>
+        <v>14423060</v>
       </c>
       <c r="N190">
-        <v>8370912</v>
+        <v>8370935</v>
       </c>
       <c r="O190">
         <v>2540056</v>
@@ -9707,7 +9707,7 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573556</v>
+        <v>573557</v>
       </c>
       <c r="E191">
         <v>207673</v>
@@ -9716,7 +9716,7 @@
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670567</v>
+        <v>8670582</v>
       </c>
       <c r="H191">
         <v>1073079</v>
@@ -9734,10 +9734,10 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14528311</v>
+        <v>14528237</v>
       </c>
       <c r="N191">
-        <v>8368442</v>
+        <v>8368466</v>
       </c>
       <c r="O191">
         <v>2551085</v>
@@ -9787,10 +9787,10 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14533086</v>
+        <v>14533012</v>
       </c>
       <c r="N192">
-        <v>8290016</v>
+        <v>8290040</v>
       </c>
       <c r="O192">
         <v>2547707</v>
@@ -9840,10 +9840,10 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761610</v>
+        <v>14761535</v>
       </c>
       <c r="N193">
-        <v>8365108</v>
+        <v>8365132</v>
       </c>
       <c r="O193">
         <v>2572355</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729051</v>
+        <v>14729052</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,10 +9893,10 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14844291</v>
+        <v>14844216</v>
       </c>
       <c r="N194">
-        <v>8387995</v>
+        <v>8388019</v>
       </c>
       <c r="O194">
         <v>2570155</v>
@@ -9946,10 +9946,10 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14889221</v>
+        <v>14889146</v>
       </c>
       <c r="N195">
-        <v>8325467</v>
+        <v>8325491</v>
       </c>
       <c r="O195">
         <v>2571044</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097745</v>
+        <v>13097750</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,10 +9999,10 @@
         <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967903</v>
+        <v>14967828</v>
       </c>
       <c r="N196">
-        <v>8319963</v>
+        <v>8319987</v>
       </c>
       <c r="O196">
         <v>2563118</v>
@@ -10052,10 +10052,10 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15090047</v>
+        <v>15089972</v>
       </c>
       <c r="N197">
-        <v>8341427</v>
+        <v>8341451</v>
       </c>
       <c r="O197">
         <v>2566573</v>
@@ -10105,10 +10105,10 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141527</v>
+        <v>15141528</v>
       </c>
       <c r="N198">
-        <v>8330316</v>
+        <v>8330317</v>
       </c>
       <c r="O198">
         <v>2567374</v>
@@ -10137,7 +10137,7 @@
         <v>214622</v>
       </c>
       <c r="F199">
-        <v>10187314</v>
+        <v>10187285</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10158,10 +10158,10 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309071</v>
+        <v>15309072</v>
       </c>
       <c r="N199">
-        <v>8356564</v>
+        <v>8356565</v>
       </c>
       <c r="O199">
         <v>2587920</v>
@@ -10187,7 +10187,7 @@
         <v>735606</v>
       </c>
       <c r="E200">
-        <v>247050</v>
+        <v>247048</v>
       </c>
       <c r="F200">
         <v>11601024</v>
@@ -10211,13 +10211,13 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440681</v>
+        <v>15440682</v>
       </c>
       <c r="N200">
-        <v>8350583</v>
+        <v>8350584</v>
       </c>
       <c r="O200">
-        <v>2599972</v>
+        <v>2599970</v>
       </c>
       <c r="P200">
         <v>3886</v>
@@ -10264,13 +10264,13 @@
         <v>133.49</v>
       </c>
       <c r="M201">
-        <v>15510455</v>
+        <v>15510456</v>
       </c>
       <c r="N201">
-        <v>8368326</v>
+        <v>8368327</v>
       </c>
       <c r="O201">
-        <v>2605547</v>
+        <v>2605545</v>
       </c>
       <c r="P201">
         <v>3887</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071191</v>
+        <v>10071192</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10317,13 +10317,13 @@
         <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673765</v>
+        <v>15673766</v>
       </c>
       <c r="N202">
-        <v>8381883</v>
+        <v>8381884</v>
       </c>
       <c r="O202">
-        <v>2635462</v>
+        <v>2635460</v>
       </c>
       <c r="P202">
         <v>3895</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851386</v>
+        <v>9851382</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -10376,7 +10376,7 @@
         <v>8380544</v>
       </c>
       <c r="O203">
-        <v>2650962</v>
+        <v>2650960</v>
       </c>
       <c r="P203">
         <v>3915</v>
@@ -10429,7 +10429,7 @@
         <v>8330361</v>
       </c>
       <c r="O204">
-        <v>2658784</v>
+        <v>2658782</v>
       </c>
       <c r="P204">
         <v>3927</v>
@@ -10482,7 +10482,7 @@
         <v>8360752</v>
       </c>
       <c r="O205">
-        <v>2687333</v>
+        <v>2687331</v>
       </c>
       <c r="P205">
         <v>3938</v>
@@ -10535,7 +10535,7 @@
         <v>8190399</v>
       </c>
       <c r="O206">
-        <v>2682387</v>
+        <v>2682385</v>
       </c>
       <c r="P206">
         <v>3943</v>
@@ -10588,7 +10588,7 @@
         <v>8167954</v>
       </c>
       <c r="O207">
-        <v>2694738</v>
+        <v>2694736</v>
       </c>
       <c r="P207">
         <v>3943</v>
@@ -10641,7 +10641,7 @@
         <v>8133267</v>
       </c>
       <c r="O208">
-        <v>2719321</v>
+        <v>2719319</v>
       </c>
       <c r="P208">
         <v>3945</v>
@@ -10694,7 +10694,7 @@
         <v>8038963</v>
       </c>
       <c r="O209">
-        <v>2707763</v>
+        <v>2707761</v>
       </c>
       <c r="P209">
         <v>3954</v>
@@ -10747,7 +10747,7 @@
         <v>7908330</v>
       </c>
       <c r="O210">
-        <v>2680328</v>
+        <v>2680326</v>
       </c>
       <c r="P210">
         <v>3955</v>
@@ -10800,7 +10800,7 @@
         <v>7873641</v>
       </c>
       <c r="O211">
-        <v>2671974</v>
+        <v>2671972</v>
       </c>
       <c r="P211">
         <v>3950</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361136</v>
+        <v>1361140</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589022</v>
+        <v>11589035</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -34403,7 +34403,7 @@
         <v>14491</v>
       </c>
       <c r="R641">
-        <v>375891</v>
+        <v>382073</v>
       </c>
     </row>
     <row r="642">
@@ -34453,13 +34453,13 @@
         <v>1476743</v>
       </c>
       <c r="P642">
-        <v>5215</v>
+        <v>5216</v>
       </c>
       <c r="Q642">
-        <v>14522</v>
+        <v>14494</v>
       </c>
       <c r="R642">
-        <v>377353</v>
+        <v>386202</v>
       </c>
     </row>
     <row r="643">
@@ -34467,49 +34467,105 @@
         <v>45107</v>
       </c>
       <c r="B643">
-        <v>1012489</v>
+        <v>1113048</v>
+      </c>
+      <c r="C643">
+        <v>1654.7</v>
       </c>
       <c r="D643">
-        <v>381565</v>
+        <v>417231</v>
       </c>
       <c r="E643">
-        <v>134495</v>
+        <v>135748</v>
       </c>
       <c r="F643">
-        <v>7120181</v>
+        <v>6939499</v>
       </c>
       <c r="G643">
-        <v>6051598</v>
+        <v>5720156</v>
       </c>
       <c r="H643">
-        <v>2536312</v>
+        <v>2439898</v>
       </c>
       <c r="I643">
-        <v>428.44</v>
+        <v>434.29</v>
       </c>
       <c r="J643">
-        <v>34.49</v>
+        <v>34.52</v>
       </c>
       <c r="K643">
-        <v>14.12</v>
+        <v>13.95</v>
       </c>
       <c r="L643">
-        <v>422.2</v>
+        <v>422.67</v>
       </c>
       <c r="M643">
-        <v>27985808</v>
+        <v>27889394</v>
       </c>
       <c r="N643">
-        <v>4784586</v>
+        <v>4820252</v>
       </c>
       <c r="O643">
-        <v>1504913</v>
+        <v>1506166</v>
       </c>
       <c r="P643">
-        <v>5242</v>
+        <v>5246</v>
       </c>
       <c r="Q643">
-        <v>14554</v>
+        <v>14518</v>
+      </c>
+      <c r="R643">
+        <v>387222</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="2">
+        <v>45138</v>
+      </c>
+      <c r="B644">
+        <v>1054535</v>
+      </c>
+      <c r="D644">
+        <v>462890</v>
+      </c>
+      <c r="E644">
+        <v>165809</v>
+      </c>
+      <c r="F644">
+        <v>8551248</v>
+      </c>
+      <c r="G644">
+        <v>6746674</v>
+      </c>
+      <c r="H644">
+        <v>2803815</v>
+      </c>
+      <c r="I644">
+        <v>423.2</v>
+      </c>
+      <c r="J644">
+        <v>34.76</v>
+      </c>
+      <c r="K644">
+        <v>14.1</v>
+      </c>
+      <c r="L644">
+        <v>425.31</v>
+      </c>
+      <c r="M644">
+        <v>28939334</v>
+      </c>
+      <c r="N644">
+        <v>4915952</v>
+      </c>
+      <c r="O644">
+        <v>1558501</v>
+      </c>
+      <c r="P644">
+        <v>5235</v>
+      </c>
+      <c r="Q644">
+        <v>14537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDP q3 update haverpull
i did it
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R645"/>
+  <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4784,13 +4784,13 @@
         <v>210662</v>
       </c>
       <c r="F98">
-        <v>13886973</v>
+        <v>13886979</v>
       </c>
       <c r="G98">
-        <v>11076407</v>
+        <v>11076413</v>
       </c>
       <c r="H98">
-        <v>904872</v>
+        <v>904873</v>
       </c>
       <c r="I98">
         <v>84.12</v>
@@ -4805,7 +4805,7 @@
         <v>79.33</v>
       </c>
       <c r="M98">
-        <v>8643094</v>
+        <v>8643095</v>
       </c>
       <c r="N98">
         <v>7816720</v>
@@ -4858,7 +4858,7 @@
         <v>79.84</v>
       </c>
       <c r="M99">
-        <v>8586181</v>
+        <v>8586182</v>
       </c>
       <c r="N99">
         <v>7675188</v>
@@ -4964,7 +4964,7 @@
         <v>80.95</v>
       </c>
       <c r="M101">
-        <v>8496278</v>
+        <v>8496279</v>
       </c>
       <c r="N101">
         <v>7630816</v>
@@ -5017,7 +5017,7 @@
         <v>81.34999999999999</v>
       </c>
       <c r="M102">
-        <v>8469981</v>
+        <v>8469982</v>
       </c>
       <c r="N102">
         <v>7605385</v>
@@ -5070,7 +5070,7 @@
         <v>81.73999999999999</v>
       </c>
       <c r="M103">
-        <v>8390319</v>
+        <v>8390320</v>
       </c>
       <c r="N103">
         <v>7610191</v>
@@ -5123,7 +5123,7 @@
         <v>82.12</v>
       </c>
       <c r="M104">
-        <v>8353744</v>
+        <v>8353745</v>
       </c>
       <c r="N104">
         <v>7610967</v>
@@ -5176,7 +5176,7 @@
         <v>82.48999999999999</v>
       </c>
       <c r="M105">
-        <v>8358621</v>
+        <v>8358622</v>
       </c>
       <c r="N105">
         <v>7677889</v>
@@ -5229,7 +5229,7 @@
         <v>82.78</v>
       </c>
       <c r="M106">
-        <v>8313964</v>
+        <v>8313965</v>
       </c>
       <c r="N106">
         <v>7636142</v>
@@ -5282,7 +5282,7 @@
         <v>83.03</v>
       </c>
       <c r="M107">
-        <v>8307259</v>
+        <v>8307260</v>
       </c>
       <c r="N107">
         <v>7633029</v>
@@ -5335,7 +5335,7 @@
         <v>83.3</v>
       </c>
       <c r="M108">
-        <v>8263908</v>
+        <v>8263909</v>
       </c>
       <c r="N108">
         <v>7603593</v>
@@ -5388,7 +5388,7 @@
         <v>83.67</v>
       </c>
       <c r="M109">
-        <v>8212243</v>
+        <v>8212244</v>
       </c>
       <c r="N109">
         <v>7568310</v>
@@ -6592,7 +6592,7 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935410</v>
+        <v>935419</v>
       </c>
       <c r="I132">
         <v>100.7</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14066957</v>
+        <v>14066966</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469409</v>
+        <v>14469419</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14605045</v>
+        <v>14605054</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690482</v>
+        <v>14690491</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14866941</v>
+        <v>14866950</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861459</v>
+        <v>14861468</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670851</v>
+        <v>14670860</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467076</v>
+        <v>14467085</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823672</v>
+        <v>823677</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14131856</v>
+        <v>14131865</v>
       </c>
       <c r="N140">
-        <v>8935508</v>
+        <v>8935513</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894152</v>
+        <v>13894161</v>
       </c>
       <c r="N141">
-        <v>8782023</v>
+        <v>8782028</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750059</v>
+        <v>13750068</v>
       </c>
       <c r="N142">
-        <v>8776291</v>
+        <v>8776296</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13621928</v>
+        <v>13621937</v>
       </c>
       <c r="N143">
-        <v>8836733</v>
+        <v>8836738</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042541</v>
+        <v>9042546</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395161</v>
+        <v>9395166</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716025</v>
+        <v>9716030</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916856</v>
+        <v>9916861</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176489</v>
+        <v>10176494</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402070</v>
+        <v>10402075</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586470</v>
+        <v>10586475</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834383</v>
+        <v>10834388</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590415</v>
+        <v>590421</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,13 +9451,13 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9817743</v>
+        <v>9817862</v>
       </c>
       <c r="H186">
-        <v>1209143</v>
+        <v>1209128</v>
       </c>
       <c r="I186">
-        <v>127.39</v>
+        <v>127.38</v>
       </c>
       <c r="J186">
         <v>32.49</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13889932</v>
+        <v>13889917</v>
       </c>
       <c r="N186">
-        <v>8211220</v>
+        <v>8211226</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13966165</v>
+        <v>13966150</v>
       </c>
       <c r="N187">
-        <v>8231211</v>
+        <v>8231217</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9575,10 +9575,10 @@
         <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177399</v>
+        <v>14177384</v>
       </c>
       <c r="N188">
-        <v>8310997</v>
+        <v>8311003</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9628,10 +9628,10 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260706</v>
+        <v>14260691</v>
       </c>
       <c r="N189">
-        <v>8315357</v>
+        <v>8315363</v>
       </c>
       <c r="O189">
         <v>2521450</v>
@@ -9681,10 +9681,10 @@
         <v>126.79</v>
       </c>
       <c r="M190">
-        <v>14423034</v>
+        <v>14423018</v>
       </c>
       <c r="N190">
-        <v>8370938</v>
+        <v>8370944</v>
       </c>
       <c r="O190">
         <v>2540056</v>
@@ -9707,7 +9707,7 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573556</v>
+        <v>573555</v>
       </c>
       <c r="E191">
         <v>207673</v>
@@ -9716,10 +9716,10 @@
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670570</v>
+        <v>8670559</v>
       </c>
       <c r="H191">
-        <v>1073079</v>
+        <v>1073078</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,10 +9734,10 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14528210</v>
+        <v>14528194</v>
       </c>
       <c r="N191">
-        <v>8368468</v>
+        <v>8368473</v>
       </c>
       <c r="O191">
         <v>2551085</v>
@@ -9787,10 +9787,10 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532984</v>
+        <v>14532968</v>
       </c>
       <c r="N192">
-        <v>8290042</v>
+        <v>8290047</v>
       </c>
       <c r="O192">
         <v>2547707</v>
@@ -9840,10 +9840,10 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761508</v>
+        <v>14761492</v>
       </c>
       <c r="N193">
-        <v>8365134</v>
+        <v>8365139</v>
       </c>
       <c r="O193">
         <v>2572355</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729050</v>
+        <v>14729048</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,10 +9893,10 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14844189</v>
+        <v>14844173</v>
       </c>
       <c r="N194">
-        <v>8388021</v>
+        <v>8388026</v>
       </c>
       <c r="O194">
         <v>2570155</v>
@@ -9946,10 +9946,10 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14889119</v>
+        <v>14889103</v>
       </c>
       <c r="N195">
-        <v>8325493</v>
+        <v>8325498</v>
       </c>
       <c r="O195">
         <v>2571044</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097756</v>
+        <v>13097754</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,10 +9999,10 @@
         <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967801</v>
+        <v>14967785</v>
       </c>
       <c r="N196">
-        <v>8319989</v>
+        <v>8319994</v>
       </c>
       <c r="O196">
         <v>2563118</v>
@@ -10052,10 +10052,10 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089945</v>
+        <v>15089929</v>
       </c>
       <c r="N197">
-        <v>8341453</v>
+        <v>8341458</v>
       </c>
       <c r="O197">
         <v>2566573</v>
@@ -10105,10 +10105,10 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141527</v>
+        <v>15141526</v>
       </c>
       <c r="N198">
-        <v>8330316</v>
+        <v>8330315</v>
       </c>
       <c r="O198">
         <v>2567374</v>
@@ -10158,10 +10158,10 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309071</v>
+        <v>15309070</v>
       </c>
       <c r="N199">
-        <v>8356564</v>
+        <v>8356563</v>
       </c>
       <c r="O199">
         <v>2587921</v>
@@ -10211,10 +10211,10 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440681</v>
+        <v>15440680</v>
       </c>
       <c r="N200">
-        <v>8350583</v>
+        <v>8350582</v>
       </c>
       <c r="O200">
         <v>2599971</v>
@@ -10264,10 +10264,10 @@
         <v>133.49</v>
       </c>
       <c r="M201">
-        <v>15510455</v>
+        <v>15510454</v>
       </c>
       <c r="N201">
-        <v>8368326</v>
+        <v>8368325</v>
       </c>
       <c r="O201">
         <v>2605546</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071183</v>
+        <v>10071179</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10317,10 +10317,10 @@
         <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673765</v>
+        <v>15673764</v>
       </c>
       <c r="N202">
-        <v>8381883</v>
+        <v>8381882</v>
       </c>
       <c r="O202">
         <v>2635461</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851370</v>
+        <v>9851360</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361140</v>
+        <v>1361139</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589038</v>
+        <v>11589036</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -34075,28 +34075,28 @@
         <v>44895</v>
       </c>
       <c r="B636">
-        <v>1008252</v>
+        <v>1008284</v>
       </c>
       <c r="C636">
         <v>1346</v>
       </c>
       <c r="D636">
-        <v>353240</v>
+        <v>353166</v>
       </c>
       <c r="E636">
-        <v>112215</v>
+        <v>112106</v>
       </c>
       <c r="F636">
-        <v>5707460</v>
+        <v>5706299</v>
       </c>
       <c r="G636">
-        <v>4583847</v>
+        <v>4582761</v>
       </c>
       <c r="H636">
-        <v>1872004</v>
+        <v>1871519</v>
       </c>
       <c r="I636">
-        <v>417.46</v>
+        <v>417.45</v>
       </c>
       <c r="J636">
         <v>30.52</v>
@@ -34108,13 +34108,13 @@
         <v>397.24</v>
       </c>
       <c r="M636">
-        <v>24210749</v>
+        <v>24210263</v>
       </c>
       <c r="N636">
-        <v>4314272</v>
+        <v>4314198</v>
       </c>
       <c r="O636">
-        <v>1586114</v>
+        <v>1586005</v>
       </c>
       <c r="P636">
         <v>5116</v>
@@ -34131,31 +34131,31 @@
         <v>44926</v>
       </c>
       <c r="B637">
-        <v>1159570</v>
+        <v>1159588</v>
       </c>
       <c r="C637">
         <v>1557.9</v>
       </c>
       <c r="D637">
-        <v>463468</v>
+        <v>463463</v>
       </c>
       <c r="E637">
-        <v>114751</v>
+        <v>114578</v>
       </c>
       <c r="F637">
-        <v>6576877</v>
+        <v>6575471</v>
       </c>
       <c r="G637">
-        <v>5404791</v>
+        <v>5403279</v>
       </c>
       <c r="H637">
-        <v>2238379</v>
+        <v>2237864</v>
       </c>
       <c r="I637">
-        <v>422.39</v>
+        <v>422.41</v>
       </c>
       <c r="J637">
-        <v>31.22</v>
+        <v>31.21</v>
       </c>
       <c r="K637">
         <v>14.22</v>
@@ -34164,13 +34164,13 @@
         <v>401.44</v>
       </c>
       <c r="M637">
-        <v>24256635</v>
+        <v>24255635</v>
       </c>
       <c r="N637">
-        <v>4362897</v>
+        <v>4362818</v>
       </c>
       <c r="O637">
-        <v>1518832</v>
+        <v>1518550</v>
       </c>
       <c r="P637">
         <v>5087</v>
@@ -34187,31 +34187,31 @@
         <v>44957</v>
       </c>
       <c r="B638">
-        <v>1226108</v>
+        <v>1226023</v>
       </c>
       <c r="C638">
         <v>1855.5</v>
       </c>
       <c r="D638">
-        <v>650635</v>
+        <v>650582</v>
       </c>
       <c r="E638">
-        <v>140555</v>
+        <v>140525</v>
       </c>
       <c r="F638">
-        <v>8985961</v>
+        <v>8985035</v>
       </c>
       <c r="G638">
-        <v>7351674</v>
+        <v>7350768</v>
       </c>
       <c r="H638">
-        <v>3117483</v>
+        <v>3117353</v>
       </c>
       <c r="I638">
-        <v>430.2</v>
+        <v>430.24</v>
       </c>
       <c r="J638">
-        <v>31.92</v>
+        <v>31.91</v>
       </c>
       <c r="K638">
         <v>13.91</v>
@@ -34220,13 +34220,13 @@
         <v>406.12</v>
       </c>
       <c r="M638">
-        <v>24738944</v>
+        <v>24737814</v>
       </c>
       <c r="N638">
-        <v>4483677</v>
+        <v>4483545</v>
       </c>
       <c r="O638">
-        <v>1481685</v>
+        <v>1481373</v>
       </c>
       <c r="P638">
         <v>5156</v>
@@ -34243,31 +34243,31 @@
         <v>44985</v>
       </c>
       <c r="B639">
-        <v>898658</v>
+        <v>898590</v>
       </c>
       <c r="C639">
         <v>1870.1</v>
       </c>
       <c r="D639">
-        <v>467290</v>
+        <v>467248</v>
       </c>
       <c r="E639">
-        <v>118686</v>
+        <v>118662</v>
       </c>
       <c r="F639">
-        <v>7772038</v>
+        <v>7771291</v>
       </c>
       <c r="G639">
-        <v>6557155</v>
+        <v>6556427</v>
       </c>
       <c r="H639">
-        <v>2820610</v>
+        <v>2820505</v>
       </c>
       <c r="I639">
-        <v>437.57</v>
+        <v>437.6</v>
       </c>
       <c r="J639">
-        <v>32.2</v>
+        <v>32.19</v>
       </c>
       <c r="K639">
         <v>13.75</v>
@@ -34276,13 +34276,13 @@
         <v>410.05</v>
       </c>
       <c r="M639">
-        <v>25144025</v>
+        <v>25142790</v>
       </c>
       <c r="N639">
-        <v>4558332</v>
+        <v>4558158</v>
       </c>
       <c r="O639">
-        <v>1461194</v>
+        <v>1460858</v>
       </c>
       <c r="P639">
         <v>5175</v>
@@ -34299,28 +34299,28 @@
         <v>45016</v>
       </c>
       <c r="B640">
-        <v>986628</v>
+        <v>986573</v>
       </c>
       <c r="C640">
         <v>1852.7</v>
       </c>
       <c r="D640">
-        <v>410627</v>
+        <v>410593</v>
       </c>
       <c r="E640">
-        <v>130480</v>
+        <v>130461</v>
       </c>
       <c r="F640">
-        <v>7973297</v>
+        <v>7972699</v>
       </c>
       <c r="G640">
-        <v>6870557</v>
+        <v>6869973</v>
       </c>
       <c r="H640">
-        <v>2977145</v>
+        <v>2977061</v>
       </c>
       <c r="I640">
-        <v>441.06</v>
+        <v>441.08</v>
       </c>
       <c r="J640">
         <v>32.73</v>
@@ -34329,16 +34329,16 @@
         <v>13.72</v>
       </c>
       <c r="L640">
-        <v>413.65</v>
+        <v>413.66</v>
       </c>
       <c r="M640">
-        <v>25580455</v>
+        <v>25579137</v>
       </c>
       <c r="N640">
-        <v>4598872</v>
+        <v>4598664</v>
       </c>
       <c r="O640">
-        <v>1423217</v>
+        <v>1422862</v>
       </c>
       <c r="P640">
         <v>5195</v>
@@ -34379,22 +34379,22 @@
         <v>435.16</v>
       </c>
       <c r="J641">
-        <v>33.72</v>
+        <v>33.71</v>
       </c>
       <c r="K641">
         <v>13.83</v>
       </c>
       <c r="L641">
-        <v>416.41</v>
+        <v>416.42</v>
       </c>
       <c r="M641">
-        <v>26308253</v>
+        <v>26306935</v>
       </c>
       <c r="N641">
-        <v>4657762</v>
+        <v>4657554</v>
       </c>
       <c r="O641">
-        <v>1446579</v>
+        <v>1446224</v>
       </c>
       <c r="P641">
         <v>5202</v>
@@ -34411,46 +34411,46 @@
         <v>45077</v>
       </c>
       <c r="B642">
-        <v>1002794</v>
+        <v>1002759</v>
       </c>
       <c r="C642">
         <v>1599.9</v>
       </c>
       <c r="D642">
-        <v>386155</v>
+        <v>386133</v>
       </c>
       <c r="E642">
-        <v>155739</v>
+        <v>155727</v>
       </c>
       <c r="F642">
-        <v>7190180</v>
+        <v>7189797</v>
       </c>
       <c r="G642">
-        <v>6150978</v>
+        <v>6150605</v>
       </c>
       <c r="H642">
-        <v>2648738</v>
+        <v>2648685</v>
       </c>
       <c r="I642">
-        <v>438.27</v>
+        <v>438.29</v>
       </c>
       <c r="J642">
-        <v>34.23</v>
+        <v>34.22</v>
       </c>
       <c r="K642">
         <v>13.93</v>
       </c>
       <c r="L642">
-        <v>419.81</v>
+        <v>419.82</v>
       </c>
       <c r="M642">
-        <v>27141875</v>
+        <v>27140503</v>
       </c>
       <c r="N642">
-        <v>4730896</v>
+        <v>4730666</v>
       </c>
       <c r="O642">
-        <v>1476743</v>
+        <v>1476376</v>
       </c>
       <c r="P642">
         <v>5216</v>
@@ -34467,46 +34467,46 @@
         <v>45107</v>
       </c>
       <c r="B643">
-        <v>1113048</v>
+        <v>1113019</v>
       </c>
       <c r="C643">
         <v>1654.7</v>
       </c>
       <c r="D643">
-        <v>417231</v>
+        <v>417214</v>
       </c>
       <c r="E643">
-        <v>135748</v>
+        <v>135738</v>
       </c>
       <c r="F643">
-        <v>6939499</v>
+        <v>6939193</v>
       </c>
       <c r="G643">
-        <v>5720156</v>
+        <v>5719857</v>
       </c>
       <c r="H643">
-        <v>2439898</v>
+        <v>2439855</v>
       </c>
       <c r="I643">
-        <v>434.29</v>
+        <v>434.31</v>
       </c>
       <c r="J643">
-        <v>34.52</v>
+        <v>34.51</v>
       </c>
       <c r="K643">
         <v>13.95</v>
       </c>
       <c r="L643">
-        <v>422.67</v>
+        <v>422.68</v>
       </c>
       <c r="M643">
-        <v>27889394</v>
+        <v>27887979</v>
       </c>
       <c r="N643">
-        <v>4820252</v>
+        <v>4820005</v>
       </c>
       <c r="O643">
-        <v>1506166</v>
+        <v>1505789</v>
       </c>
       <c r="P643">
         <v>5231</v>
@@ -34515,7 +34515,7 @@
         <v>14492</v>
       </c>
       <c r="R643">
-        <v>392077</v>
+        <v>396538</v>
       </c>
     </row>
     <row r="644">
@@ -34523,55 +34523,55 @@
         <v>45138</v>
       </c>
       <c r="B644">
-        <v>1058725</v>
+        <v>1058702</v>
       </c>
       <c r="C644">
         <v>1820.7</v>
       </c>
       <c r="D644">
-        <v>467119</v>
+        <v>467105</v>
       </c>
       <c r="E644">
-        <v>165500</v>
+        <v>165492</v>
       </c>
       <c r="F644">
-        <v>8556682</v>
+        <v>8488625</v>
       </c>
       <c r="G644">
-        <v>6749380</v>
+        <v>6749139</v>
       </c>
       <c r="H644">
-        <v>2807117</v>
+        <v>2807083</v>
       </c>
       <c r="I644">
-        <v>423.45</v>
+        <v>423.46</v>
       </c>
       <c r="J644">
-        <v>34.75</v>
+        <v>34.74</v>
       </c>
       <c r="K644">
         <v>14.09</v>
       </c>
       <c r="L644">
-        <v>425.33</v>
+        <v>425.35</v>
       </c>
       <c r="M644">
-        <v>28942636</v>
+        <v>28941187</v>
       </c>
       <c r="N644">
-        <v>4920181</v>
+        <v>4919920</v>
       </c>
       <c r="O644">
-        <v>1558192</v>
+        <v>1557807</v>
       </c>
       <c r="P644">
-        <v>5226</v>
+        <v>5243</v>
       </c>
       <c r="Q644">
-        <v>14493</v>
+        <v>14561</v>
       </c>
       <c r="R644">
-        <v>391732</v>
+        <v>397510</v>
       </c>
     </row>
     <row r="645">
@@ -34579,46 +34579,105 @@
         <v>45169</v>
       </c>
       <c r="B645">
-        <v>911799</v>
+        <v>938609</v>
+      </c>
+      <c r="C645">
+        <v>1793.4</v>
+      </c>
+      <c r="D645">
+        <v>422943</v>
       </c>
       <c r="E645">
-        <v>155688</v>
+        <v>156311</v>
       </c>
       <c r="F645">
-        <v>7499819</v>
+        <v>7609986</v>
       </c>
       <c r="G645">
-        <v>6460346</v>
+        <v>6595457</v>
       </c>
       <c r="H645">
-        <v>2744881</v>
+        <v>2808780</v>
       </c>
       <c r="I645">
-        <v>432.02</v>
+        <v>433.61</v>
       </c>
       <c r="J645">
-        <v>34.99</v>
+        <v>35</v>
       </c>
       <c r="K645">
-        <v>14.18</v>
+        <v>14.17</v>
       </c>
       <c r="L645">
-        <v>428.52</v>
+        <v>428.68</v>
       </c>
       <c r="M645">
-        <v>29670814</v>
+        <v>29733264</v>
       </c>
       <c r="N645">
-        <v>4973753</v>
+        <v>4986272</v>
       </c>
       <c r="O645">
-        <v>1595147</v>
+        <v>1595385</v>
       </c>
       <c r="P645">
-        <v>5226</v>
+        <v>5267</v>
       </c>
       <c r="Q645">
-        <v>14491</v>
+        <v>14576</v>
+      </c>
+      <c r="R645">
+        <v>397601</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="2">
+        <v>45199</v>
+      </c>
+      <c r="B646">
+        <v>739107</v>
+      </c>
+      <c r="D646">
+        <v>287345</v>
+      </c>
+      <c r="E646">
+        <v>200527</v>
+      </c>
+      <c r="F646">
+        <v>6259636</v>
+      </c>
+      <c r="G646">
+        <v>5143477</v>
+      </c>
+      <c r="H646">
+        <v>2304278</v>
+      </c>
+      <c r="I646">
+        <v>456.77</v>
+      </c>
+      <c r="J646">
+        <v>36.82</v>
+      </c>
+      <c r="K646">
+        <v>14.36</v>
+      </c>
+      <c r="L646">
+        <v>432.12</v>
+      </c>
+      <c r="M646">
+        <v>30380213</v>
+      </c>
+      <c r="N646">
+        <v>4985522</v>
+      </c>
+      <c r="O646">
+        <v>1693096</v>
+      </c>
+      <c r="P646">
+        <v>5296</v>
+      </c>
+      <c r="Q646">
+        <v>14614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drag + haver pull
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R651"/>
+  <dimension ref="A1:R652"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4784,10 +4784,10 @@
         <v>210660</v>
       </c>
       <c r="F98">
-        <v>13886948</v>
+        <v>13886949</v>
       </c>
       <c r="G98">
-        <v>11076381</v>
+        <v>11076382</v>
       </c>
       <c r="H98">
         <v>904868</v>
@@ -4805,7 +4805,7 @@
         <v>79.33</v>
       </c>
       <c r="M98">
-        <v>8643089</v>
+        <v>8643090</v>
       </c>
       <c r="N98">
         <v>7816720</v>
@@ -5123,7 +5123,7 @@
         <v>82.12</v>
       </c>
       <c r="M104">
-        <v>8353739</v>
+        <v>8353740</v>
       </c>
       <c r="N104">
         <v>7610967</v>
@@ -5335,7 +5335,7 @@
         <v>83.3</v>
       </c>
       <c r="M108">
-        <v>8263903</v>
+        <v>8263904</v>
       </c>
       <c r="N108">
         <v>7603593</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823705</v>
+        <v>823714</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7034,7 +7034,7 @@
         <v>14132126</v>
       </c>
       <c r="N140">
-        <v>8935541</v>
+        <v>8935550</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7087,7 +7087,7 @@
         <v>13894423</v>
       </c>
       <c r="N141">
-        <v>8782056</v>
+        <v>8782065</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7140,7 +7140,7 @@
         <v>13750329</v>
       </c>
       <c r="N142">
-        <v>8776324</v>
+        <v>8776333</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7193,7 +7193,7 @@
         <v>13622198</v>
       </c>
       <c r="N143">
-        <v>8836766</v>
+        <v>8836775</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042574</v>
+        <v>9042583</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395194</v>
+        <v>9395203</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716058</v>
+        <v>9716067</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916889</v>
+        <v>9916898</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176522</v>
+        <v>10176531</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402103</v>
+        <v>10402112</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586503</v>
+        <v>10586512</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834416</v>
+        <v>10834425</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -7870,7 +7870,7 @@
         <v>123.46</v>
       </c>
       <c r="J156">
-        <v>37.94</v>
+        <v>37.93</v>
       </c>
       <c r="K156">
         <v>15.57</v>
@@ -9707,19 +9707,19 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573560</v>
+        <v>573564</v>
       </c>
       <c r="E191">
-        <v>207669</v>
+        <v>207671</v>
       </c>
       <c r="F191">
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670637</v>
+        <v>8670689</v>
       </c>
       <c r="H191">
-        <v>1073110</v>
+        <v>1073112</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,13 +9734,13 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14527949</v>
+        <v>14527950</v>
       </c>
       <c r="N191">
-        <v>8368520</v>
+        <v>8368524</v>
       </c>
       <c r="O191">
-        <v>2551080</v>
+        <v>2551082</v>
       </c>
       <c r="P191">
         <v>3864</v>
@@ -9787,13 +9787,13 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532723</v>
+        <v>14532725</v>
       </c>
       <c r="N192">
-        <v>8290094</v>
+        <v>8290098</v>
       </c>
       <c r="O192">
-        <v>2547702</v>
+        <v>2547704</v>
       </c>
       <c r="P192">
         <v>3867</v>
@@ -9840,13 +9840,13 @@
         <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761247</v>
+        <v>14761249</v>
       </c>
       <c r="N193">
-        <v>8365186</v>
+        <v>8365190</v>
       </c>
       <c r="O193">
-        <v>2572350</v>
+        <v>2572352</v>
       </c>
       <c r="P193">
         <v>3862</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729042</v>
+        <v>14729044</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,13 +9893,13 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14843928</v>
+        <v>14843930</v>
       </c>
       <c r="N194">
-        <v>8388073</v>
+        <v>8388077</v>
       </c>
       <c r="O194">
-        <v>2570150</v>
+        <v>2570152</v>
       </c>
       <c r="P194">
         <v>3869</v>
@@ -9946,13 +9946,13 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14888858</v>
+        <v>14888860</v>
       </c>
       <c r="N195">
-        <v>8325545</v>
+        <v>8325549</v>
       </c>
       <c r="O195">
-        <v>2571039</v>
+        <v>2571041</v>
       </c>
       <c r="P195">
         <v>3875</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097763</v>
+        <v>13097747</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9999,13 +9999,13 @@
         <v>130.19</v>
       </c>
       <c r="M196">
-        <v>14967540</v>
+        <v>14967542</v>
       </c>
       <c r="N196">
-        <v>8320041</v>
+        <v>8320045</v>
       </c>
       <c r="O196">
-        <v>2563113</v>
+        <v>2563115</v>
       </c>
       <c r="P196">
         <v>3873</v>
@@ -10052,13 +10052,13 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089684</v>
+        <v>15089686</v>
       </c>
       <c r="N197">
-        <v>8341505</v>
+        <v>8341509</v>
       </c>
       <c r="O197">
-        <v>2566568</v>
+        <v>2566570</v>
       </c>
       <c r="P197">
         <v>3878</v>
@@ -10105,13 +10105,13 @@
         <v>131.55</v>
       </c>
       <c r="M198">
-        <v>15141559</v>
+        <v>15141561</v>
       </c>
       <c r="N198">
-        <v>8330320</v>
+        <v>8330324</v>
       </c>
       <c r="O198">
-        <v>2567369</v>
+        <v>2567371</v>
       </c>
       <c r="P198">
         <v>3884</v>
@@ -10137,7 +10137,7 @@
         <v>214626</v>
       </c>
       <c r="F199">
-        <v>10187292</v>
+        <v>10187293</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10158,13 +10158,13 @@
         <v>132.19</v>
       </c>
       <c r="M199">
-        <v>15309103</v>
+        <v>15309105</v>
       </c>
       <c r="N199">
-        <v>8356568</v>
+        <v>8356572</v>
       </c>
       <c r="O199">
-        <v>2587919</v>
+        <v>2587921</v>
       </c>
       <c r="P199">
         <v>3887</v>
@@ -10211,13 +10211,13 @@
         <v>132.87</v>
       </c>
       <c r="M200">
-        <v>15440712</v>
+        <v>15440714</v>
       </c>
       <c r="N200">
-        <v>8350587</v>
+        <v>8350591</v>
       </c>
       <c r="O200">
-        <v>2599970</v>
+        <v>2599972</v>
       </c>
       <c r="P200">
         <v>3886</v>
@@ -10264,13 +10264,13 @@
         <v>133.49</v>
       </c>
       <c r="M201">
-        <v>15510487</v>
+        <v>15510489</v>
       </c>
       <c r="N201">
-        <v>8368330</v>
+        <v>8368334</v>
       </c>
       <c r="O201">
-        <v>2605543</v>
+        <v>2605545</v>
       </c>
       <c r="P201">
         <v>3887</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071156</v>
+        <v>10071161</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10314,16 +10314,16 @@
         <v>14.46</v>
       </c>
       <c r="L202">
-        <v>134.05</v>
+        <v>134.04</v>
       </c>
       <c r="M202">
-        <v>15673797</v>
+        <v>15673799</v>
       </c>
       <c r="N202">
-        <v>8381887</v>
+        <v>8381891</v>
       </c>
       <c r="O202">
-        <v>2635460</v>
+        <v>2635462</v>
       </c>
       <c r="P202">
         <v>3895</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851297</v>
+        <v>9851303</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361148</v>
+        <v>1361125</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11589008</v>
+        <v>11588933</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -33297,10 +33297,10 @@
         <v>2479.4</v>
       </c>
       <c r="D622">
-        <v>481449</v>
+        <v>478045</v>
       </c>
       <c r="E622">
-        <v>307606</v>
+        <v>305612</v>
       </c>
       <c r="F622">
         <v>10026882</v>
@@ -33309,7 +33309,7 @@
         <v>8091977</v>
       </c>
       <c r="H622">
-        <v>2691144</v>
+        <v>2683520</v>
       </c>
       <c r="I622">
         <v>352.04</v>
@@ -33318,19 +33318,19 @@
         <v>29.08</v>
       </c>
       <c r="K622">
-        <v>20.97</v>
+        <v>20.98</v>
       </c>
       <c r="L622">
-        <v>340.08</v>
+        <v>340.1</v>
       </c>
       <c r="M622">
-        <v>58993111</v>
+        <v>58985486</v>
       </c>
       <c r="N622">
-        <v>8914437</v>
+        <v>8911033</v>
       </c>
       <c r="O622">
-        <v>8849965</v>
+        <v>8847971</v>
       </c>
       <c r="P622">
         <v>5141</v>
@@ -33371,22 +33371,22 @@
         <v>350.24</v>
       </c>
       <c r="J623">
-        <v>34.88</v>
+        <v>34.87</v>
       </c>
       <c r="K623">
-        <v>19.45</v>
+        <v>19.46</v>
       </c>
       <c r="L623">
-        <v>344.43</v>
+        <v>344.45</v>
       </c>
       <c r="M623">
-        <v>52921327</v>
+        <v>52913702</v>
       </c>
       <c r="N623">
-        <v>8507273</v>
+        <v>8503869</v>
       </c>
       <c r="O623">
-        <v>6721960</v>
+        <v>6719966</v>
       </c>
       <c r="P623">
         <v>5136</v>
@@ -33427,22 +33427,22 @@
         <v>364.68</v>
       </c>
       <c r="J624">
-        <v>39.28</v>
+        <v>39.27</v>
       </c>
       <c r="K624">
         <v>18.54</v>
       </c>
       <c r="L624">
-        <v>347.31</v>
+        <v>347.33</v>
       </c>
       <c r="M624">
-        <v>48464556</v>
+        <v>48456932</v>
       </c>
       <c r="N624">
-        <v>8095092</v>
+        <v>8091688</v>
       </c>
       <c r="O624">
-        <v>5603354</v>
+        <v>5601360</v>
       </c>
       <c r="P624">
         <v>5123</v>
@@ -33483,22 +33483,22 @@
         <v>376.45</v>
       </c>
       <c r="J625">
-        <v>40.32</v>
+        <v>40.31</v>
       </c>
       <c r="K625">
-        <v>17.79</v>
+        <v>17.8</v>
       </c>
       <c r="L625">
-        <v>349.76</v>
+        <v>349.78</v>
       </c>
       <c r="M625">
-        <v>44267580</v>
+        <v>44259956</v>
       </c>
       <c r="N625">
-        <v>7634866</v>
+        <v>7631462</v>
       </c>
       <c r="O625">
-        <v>4743936</v>
+        <v>4741942</v>
       </c>
       <c r="P625">
         <v>5121</v>
@@ -33539,22 +33539,22 @@
         <v>390.25</v>
       </c>
       <c r="J626">
-        <v>40.2</v>
+        <v>40.18</v>
       </c>
       <c r="K626">
         <v>17.28</v>
       </c>
       <c r="L626">
-        <v>352.64</v>
+        <v>352.67</v>
       </c>
       <c r="M626">
-        <v>41284386</v>
+        <v>41276761</v>
       </c>
       <c r="N626">
-        <v>7253876</v>
+        <v>7250472</v>
       </c>
       <c r="O626">
-        <v>4099872</v>
+        <v>4097878</v>
       </c>
       <c r="P626">
         <v>5094</v>
@@ -33595,22 +33595,22 @@
         <v>399.95</v>
       </c>
       <c r="J627">
-        <v>38.59</v>
+        <v>38.57</v>
       </c>
       <c r="K627">
         <v>16.82</v>
       </c>
       <c r="L627">
-        <v>355.79</v>
+        <v>355.82</v>
       </c>
       <c r="M627">
-        <v>38631758</v>
+        <v>38624133</v>
       </c>
       <c r="N627">
-        <v>6880385</v>
+        <v>6876981</v>
       </c>
       <c r="O627">
-        <v>3605843</v>
+        <v>3603849</v>
       </c>
       <c r="P627">
         <v>5083</v>
@@ -33651,22 +33651,22 @@
         <v>407.98</v>
       </c>
       <c r="J628">
-        <v>35.51</v>
+        <v>35.5</v>
       </c>
       <c r="K628">
         <v>16.51</v>
       </c>
       <c r="L628">
-        <v>359.74</v>
+        <v>359.78</v>
       </c>
       <c r="M628">
-        <v>35826011</v>
+        <v>35818386</v>
       </c>
       <c r="N628">
-        <v>6400490</v>
+        <v>6397086</v>
       </c>
       <c r="O628">
-        <v>3165532</v>
+        <v>3163538</v>
       </c>
       <c r="P628">
         <v>5065</v>
@@ -33707,22 +33707,22 @@
         <v>403.99</v>
       </c>
       <c r="J629">
-        <v>33.88</v>
+        <v>33.87</v>
       </c>
       <c r="K629">
         <v>17.38</v>
       </c>
       <c r="L629">
-        <v>363.39</v>
+        <v>363.43</v>
       </c>
       <c r="M629">
-        <v>33644296</v>
+        <v>33636671</v>
       </c>
       <c r="N629">
-        <v>5638916</v>
+        <v>5635512</v>
       </c>
       <c r="O629">
-        <v>2882179</v>
+        <v>2880185</v>
       </c>
       <c r="P629">
         <v>5080</v>
@@ -33763,22 +33763,22 @@
         <v>397.16</v>
       </c>
       <c r="J630">
-        <v>32.58</v>
+        <v>32.57</v>
       </c>
       <c r="K630">
         <v>17.39</v>
       </c>
       <c r="L630">
-        <v>367.85</v>
+        <v>367.89</v>
       </c>
       <c r="M630">
-        <v>31541846</v>
+        <v>31534221</v>
       </c>
       <c r="N630">
-        <v>5199783</v>
+        <v>5196379</v>
       </c>
       <c r="O630">
-        <v>2637209</v>
+        <v>2635215</v>
       </c>
       <c r="P630">
         <v>5096</v>
@@ -33798,7 +33798,7 @@
         <v>936213</v>
       </c>
       <c r="C631">
-        <v>1297.8</v>
+        <v>1297.2</v>
       </c>
       <c r="D631">
         <v>327875</v>
@@ -33819,22 +33819,22 @@
         <v>394.65</v>
       </c>
       <c r="J631">
-        <v>31.56</v>
+        <v>31.55</v>
       </c>
       <c r="K631">
         <v>16.92</v>
       </c>
       <c r="L631">
-        <v>372.72</v>
+        <v>372.77</v>
       </c>
       <c r="M631">
-        <v>29247780</v>
+        <v>29240156</v>
       </c>
       <c r="N631">
-        <v>4868662</v>
+        <v>4865258</v>
       </c>
       <c r="O631">
-        <v>2409588</v>
+        <v>2407594</v>
       </c>
       <c r="P631">
         <v>5103</v>
@@ -33875,22 +33875,22 @@
         <v>383.98</v>
       </c>
       <c r="J632">
-        <v>30.84</v>
+        <v>30.82</v>
       </c>
       <c r="K632">
         <v>16.42</v>
       </c>
       <c r="L632">
-        <v>377.39</v>
+        <v>377.44</v>
       </c>
       <c r="M632">
-        <v>27545447</v>
+        <v>27537822</v>
       </c>
       <c r="N632">
-        <v>4645025</v>
+        <v>4641621</v>
       </c>
       <c r="O632">
-        <v>2236797</v>
+        <v>2234803</v>
       </c>
       <c r="P632">
         <v>5129</v>
@@ -33931,22 +33931,22 @@
         <v>390.7</v>
       </c>
       <c r="J633">
-        <v>30.25</v>
+        <v>30.24</v>
       </c>
       <c r="K633">
         <v>15.62</v>
       </c>
       <c r="L633">
-        <v>382.63</v>
+        <v>382.69</v>
       </c>
       <c r="M633">
-        <v>26116251</v>
+        <v>26108626</v>
       </c>
       <c r="N633">
-        <v>4541171</v>
+        <v>4537767</v>
       </c>
       <c r="O633">
-        <v>2081428</v>
+        <v>2079434</v>
       </c>
       <c r="P633">
         <v>5139</v>
@@ -33987,7 +33987,7 @@
         <v>404.1</v>
       </c>
       <c r="J634">
-        <v>29.32</v>
+        <v>29.34</v>
       </c>
       <c r="K634">
         <v>15.41</v>
@@ -34043,7 +34043,7 @@
         <v>406.33</v>
       </c>
       <c r="J635">
-        <v>29.88</v>
+        <v>29.9</v>
       </c>
       <c r="K635">
         <v>15.05</v>
@@ -34099,7 +34099,7 @@
         <v>417.45</v>
       </c>
       <c r="J636">
-        <v>30.5</v>
+        <v>30.52</v>
       </c>
       <c r="K636">
         <v>14.54</v>
@@ -34155,7 +34155,7 @@
         <v>422.41</v>
       </c>
       <c r="J637">
-        <v>31.19</v>
+        <v>31.21</v>
       </c>
       <c r="K637">
         <v>14.22</v>
@@ -34211,7 +34211,7 @@
         <v>430.24</v>
       </c>
       <c r="J638">
-        <v>31.89</v>
+        <v>31.91</v>
       </c>
       <c r="K638">
         <v>13.91</v>
@@ -34267,7 +34267,7 @@
         <v>437.6</v>
       </c>
       <c r="J639">
-        <v>32.17</v>
+        <v>32.19</v>
       </c>
       <c r="K639">
         <v>13.75</v>
@@ -34851,7 +34851,7 @@
         <v>14711</v>
       </c>
       <c r="R649">
-        <v>446948</v>
+        <v>446894</v>
       </c>
     </row>
     <row r="650">
@@ -34901,13 +34901,13 @@
         <v>1816522</v>
       </c>
       <c r="P650">
-        <v>5423</v>
+        <v>5420</v>
       </c>
       <c r="Q650">
-        <v>14732</v>
+        <v>14742</v>
       </c>
       <c r="R650">
-        <v>442475</v>
+        <v>443767</v>
       </c>
     </row>
     <row r="651">
@@ -34915,49 +34915,105 @@
         <v>45351</v>
       </c>
       <c r="B651">
-        <v>878730</v>
+        <v>881571</v>
+      </c>
+      <c r="C651">
+        <v>2059.2</v>
       </c>
       <c r="D651">
-        <v>489893</v>
+        <v>487456</v>
       </c>
       <c r="E651">
-        <v>155281</v>
+        <v>157472</v>
       </c>
       <c r="F651">
-        <v>8517536</v>
+        <v>8524590</v>
       </c>
       <c r="G651">
-        <v>7380472</v>
+        <v>7385863</v>
       </c>
       <c r="H651">
-        <v>3332499</v>
+        <v>3339684</v>
       </c>
       <c r="I651">
-        <v>459.69</v>
+        <v>459.48</v>
       </c>
       <c r="J651">
-        <v>37.17</v>
+        <v>37.21</v>
       </c>
       <c r="K651">
-        <v>14.98</v>
+        <v>14.99</v>
       </c>
       <c r="L651">
-        <v>443.79</v>
+        <v>443.77</v>
       </c>
       <c r="M651">
-        <v>33847539</v>
+        <v>33854725</v>
       </c>
       <c r="N651">
-        <v>5184475</v>
+        <v>5182038</v>
       </c>
       <c r="O651">
-        <v>1853140</v>
+        <v>1855331</v>
       </c>
       <c r="P651">
-        <v>5428</v>
+        <v>5431</v>
       </c>
       <c r="Q651">
-        <v>14770</v>
+        <v>14784</v>
+      </c>
+      <c r="R651">
+        <v>438817</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B652">
+        <v>1180153</v>
+      </c>
+      <c r="D652">
+        <v>451949</v>
+      </c>
+      <c r="E652">
+        <v>144376</v>
+      </c>
+      <c r="F652">
+        <v>8854339</v>
+      </c>
+      <c r="G652">
+        <v>7495292</v>
+      </c>
+      <c r="H652">
+        <v>3308275</v>
+      </c>
+      <c r="I652">
+        <v>448.03</v>
+      </c>
+      <c r="J652">
+        <v>37.16</v>
+      </c>
+      <c r="K652">
+        <v>14.99</v>
+      </c>
+      <c r="L652">
+        <v>444.41</v>
+      </c>
+      <c r="M652">
+        <v>34186103</v>
+      </c>
+      <c r="N652">
+        <v>5223413</v>
+      </c>
+      <c r="O652">
+        <v>1869259</v>
+      </c>
+      <c r="P652">
+        <v>5444</v>
+      </c>
+      <c r="Q652">
+        <v>14833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
haver pull + forecast sheet prep
</commit_message>
<xml_diff>
--- a/data/monthly_state_ui.xlsx
+++ b/data/monthly_state_ui.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R654"/>
+  <dimension ref="A1:R656"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4784,13 +4784,13 @@
         <v>210661</v>
       </c>
       <c r="F98">
-        <v>13886950</v>
+        <v>13886955</v>
       </c>
       <c r="G98">
-        <v>11076383</v>
+        <v>11076388</v>
       </c>
       <c r="H98">
-        <v>904868</v>
+        <v>904869</v>
       </c>
       <c r="I98">
         <v>84.12</v>
@@ -4858,7 +4858,7 @@
         <v>79.84</v>
       </c>
       <c r="M99">
-        <v>8586177</v>
+        <v>8586178</v>
       </c>
       <c r="N99">
         <v>7675188</v>
@@ -4911,7 +4911,7 @@
         <v>80.48999999999999</v>
       </c>
       <c r="M100">
-        <v>8552550</v>
+        <v>8552551</v>
       </c>
       <c r="N100">
         <v>7655474</v>
@@ -5017,7 +5017,7 @@
         <v>81.34999999999999</v>
       </c>
       <c r="M102">
-        <v>8469976</v>
+        <v>8469977</v>
       </c>
       <c r="N102">
         <v>7605385</v>
@@ -5176,7 +5176,7 @@
         <v>82.48999999999999</v>
       </c>
       <c r="M105">
-        <v>8358617</v>
+        <v>8358618</v>
       </c>
       <c r="N105">
         <v>7677889</v>
@@ -5229,7 +5229,7 @@
         <v>82.78</v>
       </c>
       <c r="M106">
-        <v>8313959</v>
+        <v>8313960</v>
       </c>
       <c r="N106">
         <v>7636142</v>
@@ -5282,7 +5282,7 @@
         <v>83.03</v>
       </c>
       <c r="M107">
-        <v>8307254</v>
+        <v>8307255</v>
       </c>
       <c r="N107">
         <v>7633029</v>
@@ -5388,7 +5388,7 @@
         <v>83.67</v>
       </c>
       <c r="M109">
-        <v>8212238</v>
+        <v>8212239</v>
       </c>
       <c r="N109">
         <v>7568310</v>
@@ -6592,10 +6592,10 @@
         <v>9516801</v>
       </c>
       <c r="H132">
-        <v>935504</v>
+        <v>935438</v>
       </c>
       <c r="I132">
-        <v>100.71</v>
+        <v>100.7</v>
       </c>
       <c r="J132">
         <v>32.75</v>
@@ -6607,7 +6607,7 @@
         <v>99.05</v>
       </c>
       <c r="M132">
-        <v>14067051</v>
+        <v>14066985</v>
       </c>
       <c r="N132">
         <v>9919645</v>
@@ -6660,7 +6660,7 @@
         <v>99.53</v>
       </c>
       <c r="M133">
-        <v>14469504</v>
+        <v>14469437</v>
       </c>
       <c r="N133">
         <v>9992123</v>
@@ -6713,7 +6713,7 @@
         <v>100.2</v>
       </c>
       <c r="M134">
-        <v>14605139</v>
+        <v>14605072</v>
       </c>
       <c r="N134">
         <v>9946214</v>
@@ -6766,7 +6766,7 @@
         <v>100.72</v>
       </c>
       <c r="M135">
-        <v>14690576</v>
+        <v>14690509</v>
       </c>
       <c r="N135">
         <v>9890722</v>
@@ -6819,7 +6819,7 @@
         <v>101.31</v>
       </c>
       <c r="M136">
-        <v>14867035</v>
+        <v>14866968</v>
       </c>
       <c r="N136">
         <v>9919839</v>
@@ -6872,7 +6872,7 @@
         <v>101.83</v>
       </c>
       <c r="M137">
-        <v>14861553</v>
+        <v>14861486</v>
       </c>
       <c r="N137">
         <v>9793604</v>
@@ -6925,7 +6925,7 @@
         <v>102.25</v>
       </c>
       <c r="M138">
-        <v>14670945</v>
+        <v>14670878</v>
       </c>
       <c r="N138">
         <v>9476838</v>
@@ -6978,7 +6978,7 @@
         <v>102.61</v>
       </c>
       <c r="M139">
-        <v>14467170</v>
+        <v>14467103</v>
       </c>
       <c r="N139">
         <v>9214474</v>
@@ -7004,7 +7004,7 @@
         <v>2112151</v>
       </c>
       <c r="D140">
-        <v>823662</v>
+        <v>823631</v>
       </c>
       <c r="E140">
         <v>246909</v>
@@ -7031,10 +7031,10 @@
         <v>103.08</v>
       </c>
       <c r="M140">
-        <v>14131950</v>
+        <v>14131883</v>
       </c>
       <c r="N140">
-        <v>8935498</v>
+        <v>8935467</v>
       </c>
       <c r="O140">
         <v>3281695</v>
@@ -7084,10 +7084,10 @@
         <v>103.59</v>
       </c>
       <c r="M141">
-        <v>13894246</v>
+        <v>13894180</v>
       </c>
       <c r="N141">
-        <v>8782013</v>
+        <v>8781982</v>
       </c>
       <c r="O141">
         <v>3240512</v>
@@ -7137,10 +7137,10 @@
         <v>104.14</v>
       </c>
       <c r="M142">
-        <v>13750153</v>
+        <v>13750086</v>
       </c>
       <c r="N142">
-        <v>8776281</v>
+        <v>8776250</v>
       </c>
       <c r="O142">
         <v>3193123</v>
@@ -7190,10 +7190,10 @@
         <v>104.75</v>
       </c>
       <c r="M143">
-        <v>13622022</v>
+        <v>13621955</v>
       </c>
       <c r="N143">
-        <v>8836723</v>
+        <v>8836692</v>
       </c>
       <c r="O143">
         <v>3101549</v>
@@ -7246,7 +7246,7 @@
         <v>13767328</v>
       </c>
       <c r="N144">
-        <v>9042531</v>
+        <v>9042500</v>
       </c>
       <c r="O144">
         <v>3043526</v>
@@ -7299,7 +7299,7 @@
         <v>14113290</v>
       </c>
       <c r="N145">
-        <v>9395151</v>
+        <v>9395120</v>
       </c>
       <c r="O145">
         <v>2989177</v>
@@ -7352,7 +7352,7 @@
         <v>14458798</v>
       </c>
       <c r="N146">
-        <v>9716015</v>
+        <v>9715984</v>
       </c>
       <c r="O146">
         <v>2937578</v>
@@ -7405,7 +7405,7 @@
         <v>14926884</v>
       </c>
       <c r="N147">
-        <v>9916846</v>
+        <v>9916815</v>
       </c>
       <c r="O147">
         <v>2929529</v>
@@ -7458,7 +7458,7 @@
         <v>15607688</v>
       </c>
       <c r="N148">
-        <v>10176479</v>
+        <v>10176448</v>
       </c>
       <c r="O148">
         <v>2979966</v>
@@ -7511,7 +7511,7 @@
         <v>16230878</v>
       </c>
       <c r="N149">
-        <v>10402060</v>
+        <v>10402029</v>
       </c>
       <c r="O149">
         <v>3052828</v>
@@ -7564,7 +7564,7 @@
         <v>16798094</v>
       </c>
       <c r="N150">
-        <v>10586460</v>
+        <v>10586429</v>
       </c>
       <c r="O150">
         <v>3145040</v>
@@ -7617,7 +7617,7 @@
         <v>17524614</v>
       </c>
       <c r="N151">
-        <v>10834373</v>
+        <v>10834342</v>
       </c>
       <c r="O151">
         <v>3279005</v>
@@ -9442,7 +9442,7 @@
         <v>1488338</v>
       </c>
       <c r="D186">
-        <v>590475</v>
+        <v>590390</v>
       </c>
       <c r="E186">
         <v>232183</v>
@@ -9451,13 +9451,13 @@
         <v>10937527</v>
       </c>
       <c r="G186">
-        <v>9818448</v>
+        <v>9816965</v>
       </c>
       <c r="H186">
-        <v>1208792</v>
+        <v>1208882</v>
       </c>
       <c r="I186">
-        <v>127.34</v>
+        <v>127.37</v>
       </c>
       <c r="J186">
         <v>32.49</v>
@@ -9469,10 +9469,10 @@
         <v>125.18</v>
       </c>
       <c r="M186">
-        <v>13889581</v>
+        <v>13889671</v>
       </c>
       <c r="N186">
-        <v>8211280</v>
+        <v>8211195</v>
       </c>
       <c r="O186">
         <v>2510371</v>
@@ -9522,10 +9522,10 @@
         <v>125.48</v>
       </c>
       <c r="M187">
-        <v>13965814</v>
+        <v>13965904</v>
       </c>
       <c r="N187">
-        <v>8231271</v>
+        <v>8231186</v>
       </c>
       <c r="O187">
         <v>2506811</v>
@@ -9575,10 +9575,10 @@
         <v>125.89</v>
       </c>
       <c r="M188">
-        <v>14177047</v>
+        <v>14177137</v>
       </c>
       <c r="N188">
-        <v>8311057</v>
+        <v>8310972</v>
       </c>
       <c r="O188">
         <v>2528409</v>
@@ -9628,10 +9628,10 @@
         <v>126.37</v>
       </c>
       <c r="M189">
-        <v>14260355</v>
+        <v>14260445</v>
       </c>
       <c r="N189">
-        <v>8315417</v>
+        <v>8315332</v>
       </c>
       <c r="O189">
         <v>2521451</v>
@@ -9678,13 +9678,13 @@
         <v>14.06</v>
       </c>
       <c r="L190">
-        <v>126.78</v>
+        <v>126.79</v>
       </c>
       <c r="M190">
-        <v>14422682</v>
+        <v>14422772</v>
       </c>
       <c r="N190">
-        <v>8370998</v>
+        <v>8370913</v>
       </c>
       <c r="O190">
         <v>2540055</v>
@@ -9707,19 +9707,19 @@
         <v>1667576</v>
       </c>
       <c r="D191">
-        <v>573567</v>
+        <v>573569</v>
       </c>
       <c r="E191">
-        <v>207671</v>
+        <v>207672</v>
       </c>
       <c r="F191">
         <v>9966680</v>
       </c>
       <c r="G191">
-        <v>8670722</v>
+        <v>8670752</v>
       </c>
       <c r="H191">
-        <v>1073113</v>
+        <v>1073112</v>
       </c>
       <c r="I191">
         <v>128.59</v>
@@ -9734,13 +9734,13 @@
         <v>127.14</v>
       </c>
       <c r="M191">
-        <v>14527892</v>
+        <v>14527982</v>
       </c>
       <c r="N191">
-        <v>8368539</v>
+        <v>8368456</v>
       </c>
       <c r="O191">
-        <v>2551082</v>
+        <v>2551083</v>
       </c>
       <c r="P191">
         <v>3864</v>
@@ -9787,13 +9787,13 @@
         <v>127.59</v>
       </c>
       <c r="M192">
-        <v>14532667</v>
+        <v>14532757</v>
       </c>
       <c r="N192">
-        <v>8290113</v>
+        <v>8290030</v>
       </c>
       <c r="O192">
-        <v>2547704</v>
+        <v>2547705</v>
       </c>
       <c r="P192">
         <v>3867</v>
@@ -9837,16 +9837,16 @@
         <v>14.26</v>
       </c>
       <c r="L193">
-        <v>128.13</v>
+        <v>128.14</v>
       </c>
       <c r="M193">
-        <v>14761190</v>
+        <v>14761280</v>
       </c>
       <c r="N193">
-        <v>8365205</v>
+        <v>8365122</v>
       </c>
       <c r="O193">
-        <v>2572352</v>
+        <v>2572353</v>
       </c>
       <c r="P193">
         <v>3862</v>
@@ -9872,7 +9872,7 @@
         <v>235008</v>
       </c>
       <c r="F194">
-        <v>14729051</v>
+        <v>14729055</v>
       </c>
       <c r="G194">
         <v>13027499</v>
@@ -9893,13 +9893,13 @@
         <v>128.88</v>
       </c>
       <c r="M194">
-        <v>14843871</v>
+        <v>14843961</v>
       </c>
       <c r="N194">
-        <v>8388092</v>
+        <v>8388009</v>
       </c>
       <c r="O194">
-        <v>2570152</v>
+        <v>2570153</v>
       </c>
       <c r="P194">
         <v>3869</v>
@@ -9946,13 +9946,13 @@
         <v>129.54</v>
       </c>
       <c r="M195">
-        <v>14888802</v>
+        <v>14888892</v>
       </c>
       <c r="N195">
-        <v>8325564</v>
+        <v>8325481</v>
       </c>
       <c r="O195">
-        <v>2571041</v>
+        <v>2571042</v>
       </c>
       <c r="P195">
         <v>3875</v>
@@ -9978,7 +9978,7 @@
         <v>219934</v>
       </c>
       <c r="F196">
-        <v>13097726</v>
+        <v>13097739</v>
       </c>
       <c r="G196">
         <v>11730221</v>
@@ -9996,16 +9996,16 @@
         <v>14.32</v>
       </c>
       <c r="L196">
-        <v>130.19</v>
+        <v>130.2</v>
       </c>
       <c r="M196">
-        <v>14967483</v>
+        <v>14967573</v>
       </c>
       <c r="N196">
-        <v>8320060</v>
+        <v>8319977</v>
       </c>
       <c r="O196">
-        <v>2563115</v>
+        <v>2563116</v>
       </c>
       <c r="P196">
         <v>3873</v>
@@ -10052,13 +10052,13 @@
         <v>130.86</v>
       </c>
       <c r="M197">
-        <v>15089628</v>
+        <v>15089718</v>
       </c>
       <c r="N197">
-        <v>8341524</v>
+        <v>8341441</v>
       </c>
       <c r="O197">
-        <v>2566570</v>
+        <v>2566571</v>
       </c>
       <c r="P197">
         <v>3878</v>
@@ -10108,10 +10108,10 @@
         <v>15141561</v>
       </c>
       <c r="N198">
-        <v>8330327</v>
+        <v>8330329</v>
       </c>
       <c r="O198">
-        <v>2567371</v>
+        <v>2567372</v>
       </c>
       <c r="P198">
         <v>3884</v>
@@ -10134,10 +10134,10 @@
         <v>525103</v>
       </c>
       <c r="E199">
-        <v>214627</v>
+        <v>214625</v>
       </c>
       <c r="F199">
-        <v>10187293</v>
+        <v>10187276</v>
       </c>
       <c r="G199">
         <v>9028611</v>
@@ -10161,10 +10161,10 @@
         <v>15309105</v>
       </c>
       <c r="N199">
-        <v>8356575</v>
+        <v>8356577</v>
       </c>
       <c r="O199">
-        <v>2587922</v>
+        <v>2587921</v>
       </c>
       <c r="P199">
         <v>3887</v>
@@ -10187,7 +10187,7 @@
         <v>735606</v>
       </c>
       <c r="E200">
-        <v>247049</v>
+        <v>247047</v>
       </c>
       <c r="F200">
         <v>11601024</v>
@@ -10214,10 +10214,10 @@
         <v>15440715</v>
       </c>
       <c r="N200">
-        <v>8350594</v>
+        <v>8350596</v>
       </c>
       <c r="O200">
-        <v>2599973</v>
+        <v>2599970</v>
       </c>
       <c r="P200">
         <v>3886</v>
@@ -10240,7 +10240,7 @@
         <v>649662</v>
       </c>
       <c r="E201">
-        <v>210439</v>
+        <v>210438</v>
       </c>
       <c r="F201">
         <v>10189513</v>
@@ -10267,10 +10267,10 @@
         <v>15510489</v>
       </c>
       <c r="N201">
-        <v>8368337</v>
+        <v>8368339</v>
       </c>
       <c r="O201">
-        <v>2605546</v>
+        <v>2605542</v>
       </c>
       <c r="P201">
         <v>3887</v>
@@ -10296,7 +10296,7 @@
         <v>211859</v>
       </c>
       <c r="F202">
-        <v>10071173</v>
+        <v>10071177</v>
       </c>
       <c r="G202">
         <v>8724780</v>
@@ -10320,10 +10320,10 @@
         <v>15673799</v>
       </c>
       <c r="N202">
-        <v>8381894</v>
+        <v>8381896</v>
       </c>
       <c r="O202">
-        <v>2635463</v>
+        <v>2635459</v>
       </c>
       <c r="P202">
         <v>3895</v>
@@ -10349,7 +10349,7 @@
         <v>223173</v>
       </c>
       <c r="F203">
-        <v>9851299</v>
+        <v>9851292</v>
       </c>
       <c r="G203">
         <v>8695175</v>
@@ -10376,7 +10376,7 @@
         <v>8380544</v>
       </c>
       <c r="O203">
-        <v>2650965</v>
+        <v>2650960</v>
       </c>
       <c r="P203">
         <v>3915</v>
@@ -10429,7 +10429,7 @@
         <v>8330361</v>
       </c>
       <c r="O204">
-        <v>2658787</v>
+        <v>2658782</v>
       </c>
       <c r="P204">
         <v>3927</v>
@@ -10482,7 +10482,7 @@
         <v>8360752</v>
       </c>
       <c r="O205">
-        <v>2687336</v>
+        <v>2687331</v>
       </c>
       <c r="P205">
         <v>3938</v>
@@ -10535,7 +10535,7 @@
         <v>8190399</v>
       </c>
       <c r="O206">
-        <v>2682390</v>
+        <v>2682385</v>
       </c>
       <c r="P206">
         <v>3943</v>
@@ -10588,7 +10588,7 @@
         <v>8167954</v>
       </c>
       <c r="O207">
-        <v>2694741</v>
+        <v>2694736</v>
       </c>
       <c r="P207">
         <v>3943</v>
@@ -10641,7 +10641,7 @@
         <v>8133267</v>
       </c>
       <c r="O208">
-        <v>2719324</v>
+        <v>2719319</v>
       </c>
       <c r="P208">
         <v>3945</v>
@@ -10694,7 +10694,7 @@
         <v>8038963</v>
       </c>
       <c r="O209">
-        <v>2707766</v>
+        <v>2707761</v>
       </c>
       <c r="P209">
         <v>3954</v>
@@ -10747,7 +10747,7 @@
         <v>7908330</v>
       </c>
       <c r="O210">
-        <v>2680331</v>
+        <v>2680326</v>
       </c>
       <c r="P210">
         <v>3955</v>
@@ -10800,7 +10800,7 @@
         <v>7873641</v>
       </c>
       <c r="O211">
-        <v>2671972</v>
+        <v>2671969</v>
       </c>
       <c r="P211">
         <v>3950</v>
@@ -10853,7 +10853,7 @@
         <v>7781838</v>
       </c>
       <c r="O212">
-        <v>2637232</v>
+        <v>2637231</v>
       </c>
       <c r="P212">
         <v>3967</v>
@@ -11877,7 +11877,7 @@
         <v>32598</v>
       </c>
       <c r="B232">
-        <v>1361131</v>
+        <v>1361136</v>
       </c>
       <c r="D232">
         <v>652549</v>
@@ -11886,7 +11886,7 @@
         <v>176192</v>
       </c>
       <c r="F232">
-        <v>11588964</v>
+        <v>11588992</v>
       </c>
       <c r="G232">
         <v>10451849</v>
@@ -30203,7 +30203,7 @@
         <v>14347</v>
       </c>
       <c r="R566">
-        <v>266595</v>
+        <v>267025</v>
       </c>
     </row>
     <row r="567">
@@ -30259,7 +30259,7 @@
         <v>14354</v>
       </c>
       <c r="R567">
-        <v>274636</v>
+        <v>275638</v>
       </c>
     </row>
     <row r="568">
@@ -30315,7 +30315,7 @@
         <v>14356</v>
       </c>
       <c r="R568">
-        <v>274776</v>
+        <v>275640</v>
       </c>
     </row>
     <row r="569">
@@ -30371,7 +30371,7 @@
         <v>14368</v>
       </c>
       <c r="R569">
-        <v>267969</v>
+        <v>267752</v>
       </c>
     </row>
     <row r="570">
@@ -30427,7 +30427,7 @@
         <v>14358</v>
       </c>
       <c r="R570">
-        <v>275703</v>
+        <v>274777</v>
       </c>
     </row>
     <row r="571">
@@ -30483,7 +30483,7 @@
         <v>14381</v>
       </c>
       <c r="R571">
-        <v>276109</v>
+        <v>276096</v>
       </c>
     </row>
     <row r="572">
@@ -30539,7 +30539,7 @@
         <v>14390</v>
       </c>
       <c r="R572">
-        <v>275397</v>
+        <v>275423</v>
       </c>
     </row>
     <row r="573">
@@ -30595,7 +30595,7 @@
         <v>14339</v>
       </c>
       <c r="R573">
-        <v>275328</v>
+        <v>275382</v>
       </c>
     </row>
     <row r="574">
@@ -30651,7 +30651,7 @@
         <v>14390</v>
       </c>
       <c r="R574">
-        <v>275771</v>
+        <v>275268</v>
       </c>
     </row>
     <row r="575">
@@ -30707,7 +30707,7 @@
         <v>14407</v>
       </c>
       <c r="R575">
-        <v>280661</v>
+        <v>281006</v>
       </c>
     </row>
     <row r="576">
@@ -30763,7 +30763,7 @@
         <v>14427</v>
       </c>
       <c r="R576">
-        <v>284111</v>
+        <v>284408</v>
       </c>
     </row>
     <row r="577">
@@ -30819,7 +30819,7 @@
         <v>14431</v>
       </c>
       <c r="R577">
-        <v>279665</v>
+        <v>279803</v>
       </c>
     </row>
     <row r="578">
@@ -30875,7 +30875,7 @@
         <v>14428</v>
       </c>
       <c r="R578">
-        <v>278783</v>
+        <v>278536</v>
       </c>
     </row>
     <row r="579">
@@ -30931,7 +30931,7 @@
         <v>14473</v>
       </c>
       <c r="R579">
-        <v>280360</v>
+        <v>281407</v>
       </c>
     </row>
     <row r="580">
@@ -30987,7 +30987,7 @@
         <v>14471</v>
       </c>
       <c r="R580">
-        <v>282473</v>
+        <v>283722</v>
       </c>
     </row>
     <row r="581">
@@ -31043,7 +31043,7 @@
         <v>14467</v>
       </c>
       <c r="R581">
-        <v>289162</v>
+        <v>288622</v>
       </c>
     </row>
     <row r="582">
@@ -31099,7 +31099,7 @@
         <v>14482</v>
       </c>
       <c r="R582">
-        <v>290466</v>
+        <v>290059</v>
       </c>
     </row>
     <row r="583">
@@ -31155,7 +31155,7 @@
         <v>14505</v>
       </c>
       <c r="R583">
-        <v>291146</v>
+        <v>290567</v>
       </c>
     </row>
     <row r="584">
@@ -31211,7 +31211,7 @@
         <v>14462</v>
       </c>
       <c r="R584">
-        <v>294360</v>
+        <v>294781</v>
       </c>
     </row>
     <row r="585">
@@ -31267,7 +31267,7 @@
         <v>14493</v>
       </c>
       <c r="R585">
-        <v>299829</v>
+        <v>299258</v>
       </c>
     </row>
     <row r="586">
@@ -31323,7 +31323,7 @@
         <v>14486</v>
       </c>
       <c r="R586">
-        <v>287931</v>
+        <v>288216</v>
       </c>
     </row>
     <row r="587">
@@ -31379,7 +31379,7 @@
         <v>14491</v>
       </c>
       <c r="R587">
-        <v>287640</v>
+        <v>287133</v>
       </c>
     </row>
     <row r="588">
@@ -31435,7 +31435,7 @@
         <v>14499</v>
       </c>
       <c r="R588">
-        <v>285463</v>
+        <v>285853</v>
       </c>
     </row>
     <row r="589">
@@ -31491,7 +31491,7 @@
         <v>14527</v>
       </c>
       <c r="R589">
-        <v>285137</v>
+        <v>285645</v>
       </c>
     </row>
     <row r="590">
@@ -31547,7 +31547,7 @@
         <v>14527</v>
       </c>
       <c r="R590">
-        <v>295509</v>
+        <v>295719</v>
       </c>
     </row>
     <row r="591">
@@ -31603,7 +31603,7 @@
         <v>14533</v>
       </c>
       <c r="R591">
-        <v>304175</v>
+        <v>305067</v>
       </c>
     </row>
     <row r="592">
@@ -31659,7 +31659,7 @@
         <v>14567</v>
       </c>
       <c r="R592">
-        <v>305358</v>
+        <v>306010</v>
       </c>
     </row>
     <row r="593">
@@ -31715,7 +31715,7 @@
         <v>14600</v>
       </c>
       <c r="R593">
-        <v>324193</v>
+        <v>323581</v>
       </c>
     </row>
     <row r="594">
@@ -31771,7 +31771,7 @@
         <v>14583</v>
       </c>
       <c r="R594">
-        <v>320559</v>
+        <v>319247</v>
       </c>
     </row>
     <row r="595">
@@ -31827,7 +31827,7 @@
         <v>14601</v>
       </c>
       <c r="R595">
-        <v>317102</v>
+        <v>317261</v>
       </c>
     </row>
     <row r="596">
@@ -31883,7 +31883,7 @@
         <v>14552</v>
       </c>
       <c r="R596">
-        <v>324286</v>
+        <v>324076</v>
       </c>
     </row>
     <row r="597">
@@ -31939,7 +31939,7 @@
         <v>14558</v>
       </c>
       <c r="R597">
-        <v>320318</v>
+        <v>320471</v>
       </c>
     </row>
     <row r="598">
@@ -31995,7 +31995,7 @@
         <v>14582</v>
       </c>
       <c r="R598">
-        <v>326917</v>
+        <v>326913</v>
       </c>
     </row>
     <row r="599">
@@ -32051,7 +32051,7 @@
         <v>14594</v>
       </c>
       <c r="R599">
-        <v>322260</v>
+        <v>321971</v>
       </c>
     </row>
     <row r="600">
@@ -32107,7 +32107,7 @@
         <v>14619</v>
       </c>
       <c r="R600">
-        <v>323761</v>
+        <v>323942</v>
       </c>
     </row>
     <row r="601">
@@ -32163,7 +32163,7 @@
         <v>14638</v>
       </c>
       <c r="R601">
-        <v>326944</v>
+        <v>327795</v>
       </c>
     </row>
     <row r="602">
@@ -32219,7 +32219,7 @@
         <v>14666</v>
       </c>
       <c r="R602">
-        <v>342465</v>
+        <v>341963</v>
       </c>
     </row>
     <row r="603">
@@ -32275,7 +32275,7 @@
         <v>14697</v>
       </c>
       <c r="R603">
-        <v>342340</v>
+        <v>343097</v>
       </c>
     </row>
     <row r="604">
@@ -32331,7 +32331,7 @@
         <v>14692</v>
       </c>
       <c r="R604">
-        <v>345379</v>
+        <v>346286</v>
       </c>
     </row>
     <row r="605">
@@ -32387,7 +32387,7 @@
         <v>13925</v>
       </c>
       <c r="R605">
-        <v>338360</v>
+        <v>337598</v>
       </c>
     </row>
     <row r="606">
@@ -32443,7 +32443,7 @@
         <v>13460</v>
       </c>
       <c r="R606">
-        <v>347467</v>
+        <v>346584</v>
       </c>
     </row>
     <row r="607">
@@ -32499,7 +32499,7 @@
         <v>13485</v>
       </c>
       <c r="R607">
-        <v>342861</v>
+        <v>342378</v>
       </c>
     </row>
     <row r="608">
@@ -32555,7 +32555,7 @@
         <v>13559</v>
       </c>
       <c r="R608">
-        <v>336827</v>
+        <v>336713</v>
       </c>
     </row>
     <row r="609">
@@ -32611,7 +32611,7 @@
         <v>13715</v>
       </c>
       <c r="R609">
-        <v>334578</v>
+        <v>335100</v>
       </c>
     </row>
     <row r="610">
@@ -32667,7 +32667,7 @@
         <v>13718</v>
       </c>
       <c r="R610">
-        <v>335229</v>
+        <v>334831</v>
       </c>
     </row>
     <row r="611">
@@ -32723,7 +32723,7 @@
         <v>13710</v>
       </c>
       <c r="R611">
-        <v>337981</v>
+        <v>337476</v>
       </c>
     </row>
     <row r="612">
@@ -32779,7 +32779,7 @@
         <v>13711</v>
       </c>
       <c r="R612">
-        <v>342927</v>
+        <v>343612</v>
       </c>
     </row>
     <row r="613">
@@ -32835,7 +32835,7 @@
         <v>13698</v>
       </c>
       <c r="R613">
-        <v>343016</v>
+        <v>343531</v>
       </c>
     </row>
     <row r="614">
@@ -32891,7 +32891,7 @@
         <v>13746</v>
       </c>
       <c r="R614">
-        <v>345102</v>
+        <v>345096</v>
       </c>
     </row>
     <row r="615">
@@ -32947,7 +32947,7 @@
         <v>13733</v>
       </c>
       <c r="R615">
-        <v>335151</v>
+        <v>336315</v>
       </c>
     </row>
     <row r="616">
@@ -33003,7 +33003,7 @@
         <v>13781</v>
       </c>
       <c r="R616">
-        <v>336955</v>
+        <v>336681</v>
       </c>
     </row>
     <row r="617">
@@ -33059,7 +33059,7 @@
         <v>13830</v>
       </c>
       <c r="R617">
-        <v>335574</v>
+        <v>334978</v>
       </c>
     </row>
     <row r="618">
@@ -33115,7 +33115,7 @@
         <v>13854</v>
       </c>
       <c r="R618">
-        <v>338521</v>
+        <v>337801</v>
       </c>
     </row>
     <row r="619">
@@ -33171,7 +33171,7 @@
         <v>13941</v>
       </c>
       <c r="R619">
-        <v>329746</v>
+        <v>328950</v>
       </c>
     </row>
     <row r="620">
@@ -33227,7 +33227,7 @@
         <v>14023</v>
       </c>
       <c r="R620">
-        <v>328919</v>
+        <v>329615</v>
       </c>
     </row>
     <row r="621">
@@ -33283,7 +33283,7 @@
         <v>14053</v>
       </c>
       <c r="R621">
-        <v>333989</v>
+        <v>334864</v>
       </c>
     </row>
     <row r="622">
@@ -33291,28 +33291,28 @@
         <v>44469</v>
       </c>
       <c r="B622">
-        <v>1410079</v>
+        <v>1402997</v>
       </c>
       <c r="C622">
         <v>2479.4</v>
       </c>
       <c r="D622">
-        <v>478045</v>
+        <v>470934</v>
       </c>
       <c r="E622">
-        <v>305612</v>
+        <v>305938</v>
       </c>
       <c r="F622">
-        <v>10026882</v>
+        <v>10017146</v>
       </c>
       <c r="G622">
-        <v>8091977</v>
+        <v>8091653</v>
       </c>
       <c r="H622">
-        <v>2683520</v>
+        <v>2683144</v>
       </c>
       <c r="I622">
-        <v>352.04</v>
+        <v>352.03</v>
       </c>
       <c r="J622">
         <v>29.08</v>
@@ -33339,7 +33339,7 @@
         <v>14047</v>
       </c>
       <c r="R622">
-        <v>326840</v>
+        <v>326687</v>
       </c>
     </row>
     <row r="623">
@@ -33395,7 +33395,7 @@
         <v>14022</v>
       </c>
       <c r="R623">
-        <v>327373</v>
+        <v>326597</v>
       </c>
     </row>
     <row r="624">
@@ -33451,7 +33451,7 @@
         <v>14028</v>
       </c>
       <c r="R624">
-        <v>331380</v>
+        <v>331859</v>
       </c>
     </row>
     <row r="625">
@@ -33507,7 +33507,7 @@
         <v>14063</v>
       </c>
       <c r="R625">
-        <v>331492</v>
+        <v>331023</v>
       </c>
     </row>
     <row r="626">
@@ -33563,7 +33563,7 @@
         <v>14084</v>
       </c>
       <c r="R626">
-        <v>334244</v>
+        <v>336477</v>
       </c>
     </row>
     <row r="627">
@@ -33619,7 +33619,7 @@
         <v>14099</v>
       </c>
       <c r="R627">
-        <v>338416</v>
+        <v>342490</v>
       </c>
     </row>
     <row r="628">
@@ -33675,7 +33675,7 @@
         <v>14118</v>
       </c>
       <c r="R628">
-        <v>339417</v>
+        <v>342356</v>
       </c>
     </row>
     <row r="629">
@@ -33731,7 +33731,7 @@
         <v>14140</v>
       </c>
       <c r="R629">
-        <v>345062</v>
+        <v>348326</v>
       </c>
     </row>
     <row r="630">
@@ -33787,7 +33787,7 @@
         <v>14153</v>
       </c>
       <c r="R630">
-        <v>339178</v>
+        <v>343789</v>
       </c>
     </row>
     <row r="631">
@@ -33843,7 +33843,7 @@
         <v>14161</v>
       </c>
       <c r="R631">
-        <v>342484</v>
+        <v>347954</v>
       </c>
     </row>
     <row r="632">
@@ -33899,7 +33899,7 @@
         <v>14272</v>
       </c>
       <c r="R632">
-        <v>350972</v>
+        <v>359534</v>
       </c>
     </row>
     <row r="633">
@@ -33955,7 +33955,7 @@
         <v>14266</v>
       </c>
       <c r="R633">
-        <v>350286</v>
+        <v>361704</v>
       </c>
     </row>
     <row r="634">
@@ -33963,28 +33963,28 @@
         <v>44834</v>
       </c>
       <c r="B634">
-        <v>733018</v>
+        <v>733057</v>
       </c>
       <c r="C634">
         <v>1218.6</v>
       </c>
       <c r="D634">
-        <v>288095</v>
+        <v>290773</v>
       </c>
       <c r="E634">
-        <v>102816</v>
+        <v>102751</v>
       </c>
       <c r="F634">
-        <v>5707657</v>
+        <v>5708130</v>
       </c>
       <c r="G634">
-        <v>4191883</v>
+        <v>4186799</v>
       </c>
       <c r="H634">
-        <v>1657330</v>
+        <v>1656473</v>
       </c>
       <c r="I634">
-        <v>404.1</v>
+        <v>404.38</v>
       </c>
       <c r="J634">
         <v>29.51</v>
@@ -34011,7 +34011,7 @@
         <v>14260</v>
       </c>
       <c r="R634">
-        <v>355116</v>
+        <v>366800</v>
       </c>
     </row>
     <row r="635">
@@ -34067,7 +34067,7 @@
         <v>14287</v>
       </c>
       <c r="R635">
-        <v>354474</v>
+        <v>366024</v>
       </c>
     </row>
     <row r="636">
@@ -34123,7 +34123,7 @@
         <v>14328</v>
       </c>
       <c r="R636">
-        <v>359543</v>
+        <v>367116</v>
       </c>
     </row>
     <row r="637">
@@ -34179,7 +34179,7 @@
         <v>14360</v>
       </c>
       <c r="R637">
-        <v>361033</v>
+        <v>372938</v>
       </c>
     </row>
     <row r="638">
@@ -34235,7 +34235,7 @@
         <v>14402</v>
       </c>
       <c r="R638">
-        <v>364867</v>
+        <v>378357</v>
       </c>
     </row>
     <row r="639">
@@ -34291,7 +34291,7 @@
         <v>14430</v>
       </c>
       <c r="R639">
-        <v>371673</v>
+        <v>387772</v>
       </c>
     </row>
     <row r="640">
@@ -34347,7 +34347,7 @@
         <v>14457</v>
       </c>
       <c r="R640">
-        <v>374555</v>
+        <v>394738</v>
       </c>
     </row>
     <row r="641">
@@ -34403,7 +34403,7 @@
         <v>14482</v>
       </c>
       <c r="R641">
-        <v>382073</v>
+        <v>403577</v>
       </c>
     </row>
     <row r="642">
@@ -34459,7 +34459,7 @@
         <v>14508</v>
       </c>
       <c r="R642">
-        <v>388978</v>
+        <v>411117</v>
       </c>
     </row>
     <row r="643">
@@ -34515,7 +34515,7 @@
         <v>14536</v>
       </c>
       <c r="R643">
-        <v>396538</v>
+        <v>418667</v>
       </c>
     </row>
     <row r="644">
@@ -34571,7 +34571,7 @@
         <v>14564</v>
       </c>
       <c r="R644">
-        <v>404059</v>
+        <v>417761</v>
       </c>
     </row>
     <row r="645">
@@ -34627,7 +34627,7 @@
         <v>14585</v>
       </c>
       <c r="R645">
-        <v>407847</v>
+        <v>420853</v>
       </c>
     </row>
     <row r="646">
@@ -34683,7 +34683,7 @@
         <v>14612</v>
       </c>
       <c r="R646">
-        <v>418897</v>
+        <v>429575</v>
       </c>
     </row>
     <row r="647">
@@ -34739,7 +34739,7 @@
         <v>14642</v>
       </c>
       <c r="R647">
-        <v>432334</v>
+        <v>440206</v>
       </c>
     </row>
     <row r="648">
@@ -34759,7 +34759,7 @@
         <v>151099</v>
       </c>
       <c r="F648">
-        <v>6835461</v>
+        <v>6834816</v>
       </c>
       <c r="G648">
         <v>5679700</v>
@@ -34795,7 +34795,7 @@
         <v>14665</v>
       </c>
       <c r="R648">
-        <v>440095</v>
+        <v>445839</v>
       </c>
     </row>
     <row r="649">
@@ -34815,7 +34815,7 @@
         <v>159293</v>
       </c>
       <c r="F649">
-        <v>8154128</v>
+        <v>8153463</v>
       </c>
       <c r="G649">
         <v>6415249</v>
@@ -34851,7 +34851,7 @@
         <v>14711</v>
       </c>
       <c r="R649">
-        <v>446894</v>
+        <v>446422</v>
       </c>
     </row>
     <row r="650">
@@ -34859,7 +34859,7 @@
         <v>45322</v>
       </c>
       <c r="B650">
-        <v>1249757</v>
+        <v>1249509</v>
       </c>
       <c r="C650">
         <v>2050.7</v>
@@ -34871,7 +34871,7 @@
         <v>184503</v>
       </c>
       <c r="F650">
-        <v>9547638</v>
+        <v>9544615</v>
       </c>
       <c r="G650">
         <v>8366985</v>
@@ -34907,7 +34907,7 @@
         <v>14742</v>
       </c>
       <c r="R650">
-        <v>445408</v>
+        <v>442338</v>
       </c>
     </row>
     <row r="651">
@@ -34915,7 +34915,7 @@
         <v>45351</v>
       </c>
       <c r="B651">
-        <v>881185</v>
+        <v>880875</v>
       </c>
       <c r="C651">
         <v>2059.2</v>
@@ -34927,7 +34927,7 @@
         <v>157469</v>
       </c>
       <c r="F651">
-        <v>8525643</v>
+        <v>8521590</v>
       </c>
       <c r="G651">
         <v>7382243</v>
@@ -34963,7 +34963,7 @@
         <v>14776</v>
       </c>
       <c r="R651">
-        <v>448458</v>
+        <v>445503</v>
       </c>
     </row>
     <row r="652">
@@ -34971,7 +34971,7 @@
         <v>45382</v>
       </c>
       <c r="B652">
-        <v>844605</v>
+        <v>844295</v>
       </c>
       <c r="C652">
         <v>2000.4</v>
@@ -34983,10 +34983,10 @@
         <v>163774</v>
       </c>
       <c r="F652">
-        <v>8835172</v>
+        <v>8831427</v>
       </c>
       <c r="G652">
-        <v>7328647</v>
+        <v>7328646</v>
       </c>
       <c r="H652">
         <v>3287976</v>
@@ -35019,7 +35019,7 @@
         <v>14832</v>
       </c>
       <c r="R652">
-        <v>453062</v>
+        <v>450173</v>
       </c>
     </row>
     <row r="653">
@@ -35027,55 +35027,55 @@
         <v>45412</v>
       </c>
       <c r="B653">
-        <v>913252</v>
+        <v>901400</v>
       </c>
       <c r="C653">
         <v>1807.6</v>
       </c>
       <c r="D653">
-        <v>398632</v>
+        <v>383175</v>
       </c>
       <c r="E653">
-        <v>184164</v>
+        <v>185615</v>
       </c>
       <c r="F653">
-        <v>8023953</v>
+        <v>7954081</v>
       </c>
       <c r="G653">
-        <v>7141893</v>
+        <v>7093475</v>
       </c>
       <c r="H653">
-        <v>3190590</v>
+        <v>3176634</v>
       </c>
       <c r="I653">
-        <v>454.58</v>
+        <v>455.85</v>
       </c>
       <c r="J653">
-        <v>37.41</v>
+        <v>37.44</v>
       </c>
       <c r="K653">
-        <v>15.07</v>
+        <v>15.11</v>
       </c>
       <c r="L653">
-        <v>447</v>
+        <v>447.1</v>
       </c>
       <c r="M653">
-        <v>34735901</v>
+        <v>34721945</v>
       </c>
       <c r="N653">
-        <v>5248787</v>
+        <v>5233330</v>
       </c>
       <c r="O653">
-        <v>1923972</v>
+        <v>1925423</v>
       </c>
       <c r="P653">
-        <v>5450</v>
+        <v>5448</v>
       </c>
       <c r="Q653">
-        <v>14831</v>
+        <v>14828</v>
       </c>
       <c r="R653">
-        <v>451154</v>
+        <v>450938</v>
       </c>
     </row>
     <row r="654">
@@ -35083,49 +35083,161 @@
         <v>45443</v>
       </c>
       <c r="B654">
-        <v>849074</v>
+        <v>879487</v>
+      </c>
+      <c r="C654">
+        <v>1650</v>
       </c>
       <c r="D654">
-        <v>370357</v>
+        <v>378972</v>
       </c>
       <c r="E654">
-        <v>165347</v>
+        <v>168510</v>
       </c>
       <c r="F654">
-        <v>7881011</v>
+        <v>7049818</v>
       </c>
       <c r="G654">
-        <v>6680702</v>
+        <v>6013043</v>
       </c>
       <c r="H654">
-        <v>2920528</v>
+        <v>2693740</v>
       </c>
       <c r="I654">
-        <v>444.88</v>
+        <v>455.84</v>
       </c>
       <c r="J654">
-        <v>37.32</v>
+        <v>37.41</v>
       </c>
       <c r="K654">
-        <v>15.23</v>
+        <v>15.11</v>
       </c>
       <c r="L654">
-        <v>447.46</v>
+        <v>448.43</v>
       </c>
       <c r="M654">
-        <v>35008688</v>
+        <v>34767944</v>
       </c>
       <c r="N654">
-        <v>5229689</v>
+        <v>5222847</v>
       </c>
       <c r="O654">
-        <v>1933627</v>
+        <v>1938241</v>
       </c>
       <c r="P654">
-        <v>5455</v>
+        <v>5429</v>
       </c>
       <c r="Q654">
-        <v>14865</v>
+        <v>14856</v>
+      </c>
+      <c r="R654">
+        <v>449378</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B655">
+        <v>968210</v>
+      </c>
+      <c r="C655">
+        <v>1736.8</v>
+      </c>
+      <c r="D655">
+        <v>405557</v>
+      </c>
+      <c r="E655">
+        <v>159554</v>
+      </c>
+      <c r="F655">
+        <v>7674764</v>
+      </c>
+      <c r="G655">
+        <v>6015491</v>
+      </c>
+      <c r="H655">
+        <v>2623405</v>
+      </c>
+      <c r="I655">
+        <v>444.03</v>
+      </c>
+      <c r="J655">
+        <v>37.87</v>
+      </c>
+      <c r="K655">
+        <v>15.22</v>
+      </c>
+      <c r="L655">
+        <v>449.09</v>
+      </c>
+      <c r="M655">
+        <v>34952546</v>
+      </c>
+      <c r="N655">
+        <v>5207295</v>
+      </c>
+      <c r="O655">
+        <v>1962179</v>
+      </c>
+      <c r="P655">
+        <v>5445</v>
+      </c>
+      <c r="Q655">
+        <v>14881</v>
+      </c>
+      <c r="R655">
+        <v>449209</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B656">
+        <v>1066319</v>
+      </c>
+      <c r="D656">
+        <v>522165</v>
+      </c>
+      <c r="E656">
+        <v>181919</v>
+      </c>
+      <c r="F656">
+        <v>8487231</v>
+      </c>
+      <c r="G656">
+        <v>7347356</v>
+      </c>
+      <c r="H656">
+        <v>3164038</v>
+      </c>
+      <c r="I656">
+        <v>438.16</v>
+      </c>
+      <c r="J656">
+        <v>38</v>
+      </c>
+      <c r="K656">
+        <v>15.18</v>
+      </c>
+      <c r="L656">
+        <v>450.23</v>
+      </c>
+      <c r="M656">
+        <v>35310421</v>
+      </c>
+      <c r="N656">
+        <v>5259475</v>
+      </c>
+      <c r="O656">
+        <v>1978724</v>
+      </c>
+      <c r="P656">
+        <v>5452</v>
+      </c>
+      <c r="Q656">
+        <v>14890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>